<commit_message>
Added legs to emulator
</commit_message>
<xml_diff>
--- a/Sim_Emulator.xlsx
+++ b/Sim_Emulator.xlsx
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="56">
   <si>
     <t>Translational</t>
   </si>
@@ -189,6 +189,15 @@
   </si>
   <si>
     <t>Leg length</t>
+  </si>
+  <si>
+    <t>True Leg Vectors</t>
+  </si>
+  <si>
+    <t>MIN SR ANG</t>
+  </si>
+  <si>
+    <t>MAX SR ANG</t>
   </si>
 </sst>
 </file>
@@ -369,7 +378,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="49">
+  <cellXfs count="52">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -429,15 +438,11 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -447,42 +452,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -499,6 +468,55 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -981,6 +999,133 @@
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000012-E1F4-4F1A-A470-60C2A1124C16}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="4"/>
+          <c:tx>
+            <c:v>True Legs</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$N$62:$N$78</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="17"/>
+                <c:pt idx="0">
+                  <c:v>158.83625015431414</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>103.04907607912567</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>148.66436998144388</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>56.701113987652391</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>-81.313090870677314</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>41.50496753893048</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>-122.80367652117502</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>-147.54602973993948</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>-77.523159283636829</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>-144.5540436180562</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>-25.860693460268838</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>90.844915752287093</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$O$62:$O$78</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="17"/>
+                <c:pt idx="0">
+                  <c:v>21.843710432906658</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>121.75152316959309</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>37.503063171720314</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>193.10304076329146</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>37.503063171720264</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>193.10304076329146</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>21.843710432906644</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>121.75152316959307</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>-47.864502755615796</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>117.14543606711544</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>-47.864502755615774</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>117.14543606711545</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-C004-4F06-8F46-9010CCF09B3B}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -2737,7 +2882,7 @@
   <dimension ref="A1:AC114"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="54" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="U16" sqref="U16"/>
+      <selection activeCell="L57" sqref="L57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2777,7 +2922,7 @@
       </c>
     </row>
     <row r="2" spans="1:29" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="29" t="s">
+      <c r="A2" s="27" t="s">
         <v>7</v>
       </c>
       <c r="B2" s="6">
@@ -2802,18 +2947,18 @@
         <f t="shared" ref="G2:G7" si="1">(-0.35*C2)+E2</f>
         <v>5.9475624695284148</v>
       </c>
-      <c r="T2" s="38" t="s">
+      <c r="T2" s="35" t="s">
         <v>12</v>
       </c>
-      <c r="U2" s="40"/>
-      <c r="W2" s="38" t="s">
+      <c r="U2" s="36"/>
+      <c r="W2" s="35" t="s">
         <v>13</v>
       </c>
-      <c r="X2" s="39"/>
-      <c r="Y2" s="40"/>
+      <c r="X2" s="38"/>
+      <c r="Y2" s="36"/>
     </row>
     <row r="3" spans="1:29" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="30"/>
+      <c r="A3" s="28"/>
       <c r="B3" s="6">
         <v>2</v>
       </c>
@@ -2856,7 +3001,7 @@
       </c>
     </row>
     <row r="4" spans="1:29" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="30"/>
+      <c r="A4" s="28"/>
       <c r="B4" s="6">
         <v>3</v>
       </c>
@@ -2899,7 +3044,7 @@
       </c>
     </row>
     <row r="5" spans="1:29" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="30"/>
+      <c r="A5" s="28"/>
       <c r="B5" s="6">
         <v>4</v>
       </c>
@@ -2942,7 +3087,7 @@
       </c>
     </row>
     <row r="6" spans="1:29" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="30"/>
+      <c r="A6" s="28"/>
       <c r="B6" s="6">
         <v>5</v>
       </c>
@@ -2967,7 +3112,7 @@
       </c>
     </row>
     <row r="7" spans="1:29" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="30"/>
+      <c r="A7" s="28"/>
       <c r="B7" s="6">
         <v>6</v>
       </c>
@@ -2992,7 +3137,7 @@
       </c>
     </row>
     <row r="8" spans="1:29" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="31"/>
+      <c r="A8" s="29"/>
       <c r="B8" s="6" t="s">
         <v>39</v>
       </c>
@@ -3007,19 +3152,19 @@
         <f>(-0.35*C2)+E2</f>
         <v>5.9475624695284148</v>
       </c>
-      <c r="T8" s="38" t="s">
+      <c r="T8" s="35" t="s">
         <v>24</v>
       </c>
-      <c r="U8" s="40"/>
-      <c r="W8" s="44" t="s">
+      <c r="U8" s="36"/>
+      <c r="W8" s="30" t="s">
         <v>35</v>
       </c>
-      <c r="X8" s="45"/>
-      <c r="Y8" s="45"/>
-      <c r="Z8" s="45"/>
-      <c r="AA8" s="45"/>
-      <c r="AB8" s="45"/>
-      <c r="AC8" s="46"/>
+      <c r="X8" s="31"/>
+      <c r="Y8" s="31"/>
+      <c r="Z8" s="31"/>
+      <c r="AA8" s="31"/>
+      <c r="AB8" s="31"/>
+      <c r="AC8" s="32"/>
     </row>
     <row r="9" spans="1:29" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="20"/>
@@ -3056,7 +3201,7 @@
       </c>
     </row>
     <row r="10" spans="1:29" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="37" t="s">
+      <c r="A10" s="26" t="s">
         <v>10</v>
       </c>
       <c r="B10" s="6">
@@ -3110,7 +3255,7 @@
       </c>
     </row>
     <row r="11" spans="1:29" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="37"/>
+      <c r="A11" s="26"/>
       <c r="B11" s="6"/>
       <c r="C11" s="11"/>
       <c r="D11" s="11"/>
@@ -3152,7 +3297,7 @@
       </c>
     </row>
     <row r="12" spans="1:29" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="37"/>
+      <c r="A12" s="26"/>
       <c r="B12" s="6">
         <v>2</v>
       </c>
@@ -3210,7 +3355,7 @@
       </c>
     </row>
     <row r="13" spans="1:29" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="37"/>
+      <c r="A13" s="26"/>
       <c r="B13" s="6"/>
       <c r="C13" s="11"/>
       <c r="D13" s="11"/>
@@ -3246,7 +3391,7 @@
       </c>
     </row>
     <row r="14" spans="1:29" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="37"/>
+      <c r="A14" s="26"/>
       <c r="B14" s="6">
         <v>3</v>
       </c>
@@ -3304,7 +3449,7 @@
       </c>
     </row>
     <row r="15" spans="1:29" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="37"/>
+      <c r="A15" s="26"/>
       <c r="B15" s="6"/>
       <c r="C15" s="11"/>
       <c r="D15" s="11"/>
@@ -3346,7 +3491,7 @@
       </c>
     </row>
     <row r="16" spans="1:29" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="37"/>
+      <c r="A16" s="26"/>
       <c r="B16" s="6">
         <v>4</v>
       </c>
@@ -3398,7 +3543,7 @@
       </c>
     </row>
     <row r="17" spans="1:29" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="37"/>
+      <c r="A17" s="26"/>
       <c r="B17" s="6"/>
       <c r="C17" s="11"/>
       <c r="D17" s="11"/>
@@ -3440,7 +3585,7 @@
       </c>
     </row>
     <row r="18" spans="1:29" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="37"/>
+      <c r="A18" s="26"/>
       <c r="B18" s="6">
         <v>5</v>
       </c>
@@ -3463,18 +3608,30 @@
         <f>(-0.35*C18)+E18</f>
         <v>-26.854563932884556</v>
       </c>
+      <c r="T18" s="49" t="s">
+        <v>54</v>
+      </c>
+      <c r="U18" s="50">
+        <v>-90</v>
+      </c>
     </row>
     <row r="19" spans="1:29" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="37"/>
+      <c r="A19" s="26"/>
       <c r="B19" s="6"/>
       <c r="C19" s="11"/>
       <c r="D19" s="11"/>
       <c r="E19" s="11"/>
       <c r="F19" s="11"/>
       <c r="G19" s="11"/>
+      <c r="T19" s="49" t="s">
+        <v>55</v>
+      </c>
+      <c r="U19" s="50">
+        <v>90</v>
+      </c>
     </row>
     <row r="20" spans="1:29" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="37"/>
+      <c r="A20" s="26"/>
       <c r="B20" s="6">
         <v>6</v>
       </c>
@@ -3497,19 +3654,19 @@
         <f>(-0.35*C20)+E20</f>
         <v>-26.854563932884545</v>
       </c>
-      <c r="T20" s="47" t="s">
+      <c r="T20" s="33" t="s">
         <v>36</v>
       </c>
-      <c r="U20" s="48"/>
-      <c r="W20" s="37" t="s">
+      <c r="U20" s="34"/>
+      <c r="W20" s="26" t="s">
         <v>0</v>
       </c>
-      <c r="X20" s="37"/>
-      <c r="Z20" s="37" t="s">
+      <c r="X20" s="26"/>
+      <c r="Z20" s="26" t="s">
         <v>1</v>
       </c>
-      <c r="AA20" s="37"/>
-      <c r="AB20" s="37"/>
+      <c r="AA20" s="26"/>
+      <c r="AB20" s="26"/>
     </row>
     <row r="21" spans="1:29" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="20"/>
@@ -3525,11 +3682,11 @@
       <c r="U21" s="5">
         <v>0</v>
       </c>
-      <c r="W21" s="41">
+      <c r="W21" s="39">
         <f>U25+U3</f>
         <v>0</v>
       </c>
-      <c r="X21" s="42"/>
+      <c r="X21" s="40"/>
       <c r="Z21" s="15">
         <f>COS(Y5)*COS(Y4)</f>
         <v>1</v>
@@ -3544,7 +3701,7 @@
       </c>
     </row>
     <row r="22" spans="1:29" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="29" t="s">
+      <c r="A22" s="27" t="s">
         <v>11</v>
       </c>
       <c r="B22" s="6">
@@ -3576,11 +3733,11 @@
       <c r="U22" s="5">
         <v>0</v>
       </c>
-      <c r="W22" s="35">
+      <c r="W22" s="41">
         <f>U26+U4</f>
         <v>0</v>
       </c>
-      <c r="X22" s="43"/>
+      <c r="X22" s="42"/>
       <c r="Z22" s="5">
         <f>SIN(Y5)*COS(Y4)</f>
         <v>0</v>
@@ -3595,7 +3752,7 @@
       </c>
     </row>
     <row r="23" spans="1:29" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="30"/>
+      <c r="A23" s="28"/>
       <c r="B23" s="6">
         <v>2</v>
       </c>
@@ -3625,11 +3782,11 @@
       <c r="U23" s="5">
         <v>0</v>
       </c>
-      <c r="W23" s="41">
+      <c r="W23" s="39">
         <f>U27+U5</f>
         <v>144</v>
       </c>
-      <c r="X23" s="41"/>
+      <c r="X23" s="39"/>
       <c r="Z23" s="5">
         <f>-SIN(Y4)</f>
         <v>0</v>
@@ -3644,7 +3801,7 @@
       </c>
     </row>
     <row r="24" spans="1:29" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="30"/>
+      <c r="A24" s="28"/>
       <c r="B24" s="6">
         <v>3</v>
       </c>
@@ -3668,10 +3825,10 @@
         <f t="shared" si="8"/>
         <v>193.10304076329146</v>
       </c>
-      <c r="T24" s="47" t="s">
+      <c r="T24" s="33" t="s">
         <v>37</v>
       </c>
-      <c r="U24" s="48"/>
+      <c r="U24" s="34"/>
       <c r="W24" s="19"/>
       <c r="X24" s="23"/>
       <c r="Y24" s="17"/>
@@ -3680,7 +3837,7 @@
       <c r="AB24" s="14"/>
     </row>
     <row r="25" spans="1:29" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="30"/>
+      <c r="A25" s="28"/>
       <c r="B25" s="6">
         <v>4</v>
       </c>
@@ -3712,7 +3869,7 @@
       </c>
     </row>
     <row r="26" spans="1:29" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="30"/>
+      <c r="A26" s="28"/>
       <c r="B26" s="6">
         <v>5</v>
       </c>
@@ -3744,7 +3901,7 @@
       </c>
     </row>
     <row r="27" spans="1:29" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="30"/>
+      <c r="A27" s="28"/>
       <c r="B27" s="6">
         <v>6</v>
       </c>
@@ -3783,7 +3940,7 @@
       <c r="AC27" s="24"/>
     </row>
     <row r="28" spans="1:29" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="31"/>
+      <c r="A28" s="29"/>
       <c r="B28" s="6" t="s">
         <v>39</v>
       </c>
@@ -3811,35 +3968,35 @@
       <c r="J29" s="17"/>
     </row>
     <row r="30" spans="1:29" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="29" t="s">
+      <c r="A30" s="27" t="s">
         <v>52</v>
       </c>
       <c r="B30" s="6">
         <v>1</v>
       </c>
-      <c r="C30" s="32">
+      <c r="C30" s="46">
         <f>SQRT(POWER($C22-$C2,2)+POWER($D22-$D2,2)+POWER($E22-$E2,2))</f>
         <v>165.06110118251149</v>
       </c>
-      <c r="D30" s="33"/>
-      <c r="E30" s="33"/>
-      <c r="F30" s="33"/>
-      <c r="G30" s="34"/>
+      <c r="D30" s="47"/>
+      <c r="E30" s="47"/>
+      <c r="F30" s="47"/>
+      <c r="G30" s="48"/>
     </row>
     <row r="31" spans="1:29" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="30"/>
+      <c r="A31" s="28"/>
       <c r="B31" s="6">
         <v>2</v>
       </c>
-      <c r="C31" s="32">
+      <c r="C31" s="46">
         <f>SQRT(POWER($C23-$C3,2)+POWER($D23-$D3,2)+POWER($E23-$E3,2))</f>
         <v>165.06110118251149</v>
       </c>
-      <c r="D31" s="33"/>
-      <c r="E31" s="33"/>
-      <c r="F31" s="33"/>
-      <c r="G31" s="34"/>
-      <c r="T31" s="37" t="s">
+      <c r="D31" s="47"/>
+      <c r="E31" s="47"/>
+      <c r="F31" s="47"/>
+      <c r="G31" s="48"/>
+      <c r="T31" s="26" t="s">
         <v>34</v>
       </c>
       <c r="U31" s="6">
@@ -3851,19 +4008,19 @@
       </c>
     </row>
     <row r="32" spans="1:29" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="30"/>
+      <c r="A32" s="28"/>
       <c r="B32" s="6">
         <v>3</v>
       </c>
-      <c r="C32" s="32">
+      <c r="C32" s="46">
         <f t="shared" ref="C32:C34" si="9">SQRT(POWER($C24-$C4,2)+POWER($D24-$D4,2)+POWER($E24-$E4,2))</f>
         <v>165.06110118251144</v>
       </c>
-      <c r="D32" s="33"/>
-      <c r="E32" s="33"/>
-      <c r="F32" s="33"/>
-      <c r="G32" s="34"/>
-      <c r="T32" s="37"/>
+      <c r="D32" s="47"/>
+      <c r="E32" s="47"/>
+      <c r="F32" s="47"/>
+      <c r="G32" s="48"/>
+      <c r="T32" s="26"/>
       <c r="U32" s="6">
         <v>2</v>
       </c>
@@ -3873,19 +4030,19 @@
       </c>
     </row>
     <row r="33" spans="1:29" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="30"/>
+      <c r="A33" s="28"/>
       <c r="B33" s="6">
         <v>4</v>
       </c>
-      <c r="C33" s="32">
+      <c r="C33" s="46">
         <f t="shared" si="9"/>
         <v>165.06110118251149</v>
       </c>
-      <c r="D33" s="33"/>
-      <c r="E33" s="33"/>
-      <c r="F33" s="33"/>
-      <c r="G33" s="34"/>
-      <c r="T33" s="37"/>
+      <c r="D33" s="47"/>
+      <c r="E33" s="47"/>
+      <c r="F33" s="47"/>
+      <c r="G33" s="48"/>
+      <c r="T33" s="26"/>
       <c r="U33" s="6">
         <v>3</v>
       </c>
@@ -3895,19 +4052,19 @@
       </c>
     </row>
     <row r="34" spans="1:29" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="30"/>
+      <c r="A34" s="28"/>
       <c r="B34" s="6">
         <v>5</v>
       </c>
-      <c r="C34" s="32">
+      <c r="C34" s="46">
         <f t="shared" si="9"/>
         <v>165.06110118251146</v>
       </c>
-      <c r="D34" s="33"/>
-      <c r="E34" s="33"/>
-      <c r="F34" s="33"/>
-      <c r="G34" s="34"/>
-      <c r="T34" s="37"/>
+      <c r="D34" s="47"/>
+      <c r="E34" s="47"/>
+      <c r="F34" s="47"/>
+      <c r="G34" s="48"/>
+      <c r="T34" s="26"/>
       <c r="U34" s="6">
         <v>4</v>
       </c>
@@ -3917,19 +4074,19 @@
       </c>
     </row>
     <row r="35" spans="1:29" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="31"/>
+      <c r="A35" s="29"/>
       <c r="B35" s="6">
         <v>6</v>
       </c>
-      <c r="C35" s="32">
+      <c r="C35" s="46">
         <f>SQRT(POWER($C27-$C7,2)+POWER($D27-$D7,2)+POWER($E27-$E7,2))</f>
         <v>165.06110118251146</v>
       </c>
-      <c r="D35" s="33"/>
-      <c r="E35" s="33"/>
-      <c r="F35" s="33"/>
-      <c r="G35" s="34"/>
-      <c r="T35" s="37"/>
+      <c r="D35" s="47"/>
+      <c r="E35" s="47"/>
+      <c r="F35" s="47"/>
+      <c r="G35" s="48"/>
+      <c r="T35" s="26"/>
       <c r="U35" s="6">
         <v>5</v>
       </c>
@@ -3946,7 +4103,7 @@
       <c r="E36" s="21"/>
       <c r="F36" s="21"/>
       <c r="G36" s="21"/>
-      <c r="T36" s="37"/>
+      <c r="T36" s="26"/>
       <c r="U36" s="6">
         <v>6</v>
       </c>
@@ -3956,8 +4113,8 @@
       </c>
     </row>
     <row r="37" spans="1:29" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A37" s="29" t="s">
-        <v>51</v>
+      <c r="A37" s="27" t="s">
+        <v>53</v>
       </c>
       <c r="B37" s="6">
         <v>1</v>
@@ -3982,7 +4139,7 @@
         <f>G22</f>
         <v>121.75152316959309</v>
       </c>
-      <c r="T37" s="37" t="s">
+      <c r="T37" s="26" t="s">
         <v>40</v>
       </c>
       <c r="U37" s="6">
@@ -3994,7 +4151,7 @@
       </c>
     </row>
     <row r="38" spans="1:29" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A38" s="30"/>
+      <c r="A38" s="28"/>
       <c r="B38" s="6"/>
       <c r="C38" s="11">
         <f>C2</f>
@@ -4016,7 +4173,7 @@
         <f>G2</f>
         <v>5.9475624695284148</v>
       </c>
-      <c r="T38" s="37"/>
+      <c r="T38" s="26"/>
       <c r="U38" s="6">
         <v>2</v>
       </c>
@@ -4026,14 +4183,14 @@
       </c>
     </row>
     <row r="39" spans="1:29" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A39" s="30"/>
+      <c r="A39" s="28"/>
       <c r="B39" s="6"/>
       <c r="C39" s="11"/>
       <c r="D39" s="11"/>
       <c r="E39" s="11"/>
       <c r="F39" s="11"/>
       <c r="G39" s="11"/>
-      <c r="T39" s="37"/>
+      <c r="T39" s="26"/>
       <c r="U39" s="6">
         <v>3</v>
       </c>
@@ -4043,7 +4200,7 @@
       </c>
     </row>
     <row r="40" spans="1:29" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A40" s="30"/>
+      <c r="A40" s="28"/>
       <c r="B40" s="6">
         <v>2</v>
       </c>
@@ -4067,7 +4224,7 @@
         <f>G23</f>
         <v>193.10304076329146</v>
       </c>
-      <c r="T40" s="37"/>
+      <c r="T40" s="26"/>
       <c r="U40" s="6">
         <v>4</v>
       </c>
@@ -4077,7 +4234,7 @@
       </c>
     </row>
     <row r="41" spans="1:29" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A41" s="30"/>
+      <c r="A41" s="28"/>
       <c r="B41" s="6"/>
       <c r="C41" s="11">
         <f>C3</f>
@@ -4099,7 +4256,7 @@
         <f>G3</f>
         <v>33.675639555383249</v>
       </c>
-      <c r="T41" s="37"/>
+      <c r="T41" s="26"/>
       <c r="U41" s="6">
         <v>5</v>
       </c>
@@ -4109,14 +4266,14 @@
       </c>
     </row>
     <row r="42" spans="1:29" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A42" s="30"/>
+      <c r="A42" s="28"/>
       <c r="B42" s="6"/>
       <c r="C42" s="11"/>
       <c r="D42" s="11"/>
       <c r="E42" s="11"/>
       <c r="F42" s="11"/>
       <c r="G42" s="11"/>
-      <c r="T42" s="37"/>
+      <c r="T42" s="26"/>
       <c r="U42" s="6">
         <v>6</v>
       </c>
@@ -4126,7 +4283,7 @@
       </c>
     </row>
     <row r="43" spans="1:29" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A43" s="30"/>
+      <c r="A43" s="28"/>
       <c r="B43" s="6">
         <v>3</v>
       </c>
@@ -4150,7 +4307,7 @@
         <f>G24</f>
         <v>193.10304076329146</v>
       </c>
-      <c r="T43" s="37" t="s">
+      <c r="T43" s="26" t="s">
         <v>41</v>
       </c>
       <c r="U43" s="6">
@@ -4162,7 +4319,7 @@
       </c>
     </row>
     <row r="44" spans="1:29" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A44" s="30"/>
+      <c r="A44" s="28"/>
       <c r="B44" s="6"/>
       <c r="C44" s="11">
         <f>C4</f>
@@ -4184,7 +4341,7 @@
         <f>G4</f>
         <v>33.67563955538327</v>
       </c>
-      <c r="T44" s="37"/>
+      <c r="T44" s="26"/>
       <c r="U44" s="6">
         <v>2</v>
       </c>
@@ -4194,14 +4351,14 @@
       </c>
     </row>
     <row r="45" spans="1:29" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A45" s="30"/>
+      <c r="A45" s="28"/>
       <c r="B45" s="6"/>
       <c r="C45" s="11"/>
       <c r="D45" s="11"/>
       <c r="E45" s="11"/>
       <c r="F45" s="11"/>
       <c r="G45" s="11"/>
-      <c r="T45" s="37"/>
+      <c r="T45" s="26"/>
       <c r="U45" s="6">
         <v>3</v>
       </c>
@@ -4211,7 +4368,7 @@
       </c>
     </row>
     <row r="46" spans="1:29" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A46" s="30"/>
+      <c r="A46" s="28"/>
       <c r="B46" s="6">
         <v>4</v>
       </c>
@@ -4235,7 +4392,7 @@
         <f>G25</f>
         <v>121.75152316959307</v>
       </c>
-      <c r="T46" s="37"/>
+      <c r="T46" s="26"/>
       <c r="U46" s="6">
         <v>4</v>
       </c>
@@ -4245,7 +4402,7 @@
       </c>
     </row>
     <row r="47" spans="1:29" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A47" s="30"/>
+      <c r="A47" s="28"/>
       <c r="B47" s="6"/>
       <c r="C47" s="11">
         <f>C5</f>
@@ -4267,7 +4424,7 @@
         <f>G5</f>
         <v>5.9475624695283997</v>
       </c>
-      <c r="T47" s="37"/>
+      <c r="T47" s="26"/>
       <c r="U47" s="6">
         <v>5</v>
       </c>
@@ -4277,14 +4434,14 @@
       </c>
     </row>
     <row r="48" spans="1:29" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A48" s="30"/>
+      <c r="A48" s="28"/>
       <c r="B48" s="6"/>
       <c r="C48" s="11"/>
       <c r="D48" s="11"/>
       <c r="E48" s="11"/>
       <c r="F48" s="11"/>
       <c r="G48" s="11"/>
-      <c r="T48" s="37"/>
+      <c r="T48" s="26"/>
       <c r="U48" s="6">
         <v>6</v>
       </c>
@@ -4312,7 +4469,7 @@
       </c>
     </row>
     <row r="49" spans="1:29" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A49" s="30"/>
+      <c r="A49" s="28"/>
       <c r="B49" s="6">
         <v>5</v>
       </c>
@@ -4356,7 +4513,7 @@
       </c>
     </row>
     <row r="50" spans="1:29" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A50" s="30"/>
+      <c r="A50" s="28"/>
       <c r="B50" s="6"/>
       <c r="C50" s="11">
         <f>C6</f>
@@ -4380,7 +4537,7 @@
       </c>
     </row>
     <row r="51" spans="1:29" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A51" s="30"/>
+      <c r="A51" s="28"/>
       <c r="B51" s="6"/>
       <c r="C51" s="11"/>
       <c r="D51" s="11"/>
@@ -4389,7 +4546,7 @@
       <c r="G51" s="11"/>
     </row>
     <row r="52" spans="1:29" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A52" s="30"/>
+      <c r="A52" s="28"/>
       <c r="B52" s="6">
         <v>6</v>
       </c>
@@ -4415,7 +4572,7 @@
       </c>
     </row>
     <row r="53" spans="1:29" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A53" s="31"/>
+      <c r="A53" s="29"/>
       <c r="B53" s="6"/>
       <c r="C53" s="11">
         <f>C7</f>
@@ -4448,108 +4605,126 @@
       <c r="G54" s="22"/>
     </row>
     <row r="55" spans="1:29" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A55" s="29" t="s">
+      <c r="A55" s="27" t="s">
         <v>38</v>
       </c>
       <c r="B55" s="6">
         <v>1</v>
       </c>
-      <c r="C55" s="35">
+      <c r="C55" s="41">
         <f t="shared" ref="C55:C60" si="11">ASIN(V31/(SQRT(POWER(V37,2)+POWER(V43,2))))-ATAN(V43/V37)</f>
         <v>9.5832207228700061E-2</v>
       </c>
-      <c r="D55" s="36"/>
-      <c r="E55" s="36">
+      <c r="D55" s="37"/>
+      <c r="E55" s="37">
         <f t="shared" ref="E55:E60" si="12">DEGREES(C55)</f>
         <v>5.4907810156276122</v>
       </c>
-      <c r="F55" s="36"/>
-      <c r="G55" s="25"/>
+      <c r="F55" s="37"/>
+      <c r="G55" s="51">
+        <f>((E55-$U$18)*($U$11-$U$10))/($U$19-$U$18)+$U$10</f>
+        <v>388.72695253906903</v>
+      </c>
     </row>
     <row r="56" spans="1:29" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A56" s="30"/>
+      <c r="A56" s="28"/>
       <c r="B56" s="6">
         <v>2</v>
       </c>
-      <c r="C56" s="35">
+      <c r="C56" s="41">
         <f t="shared" si="11"/>
         <v>9.5832207228699617E-2</v>
       </c>
-      <c r="D56" s="36"/>
-      <c r="E56" s="36">
+      <c r="D56" s="37"/>
+      <c r="E56" s="37">
         <f t="shared" si="12"/>
         <v>5.4907810156275874</v>
       </c>
-      <c r="F56" s="36"/>
-      <c r="G56" s="25"/>
+      <c r="F56" s="37"/>
+      <c r="G56" s="51">
+        <f t="shared" ref="G56:G60" si="13">((E56-$U$18)*($U$11-$U$10))/($U$19-$U$18)+$U$10</f>
+        <v>388.72695253906898</v>
+      </c>
     </row>
     <row r="57" spans="1:29" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A57" s="30"/>
+      <c r="A57" s="28"/>
       <c r="B57" s="6">
         <v>3</v>
       </c>
-      <c r="C57" s="35">
+      <c r="C57" s="41">
         <f t="shared" si="11"/>
         <v>9.5832207228697841E-2</v>
       </c>
-      <c r="D57" s="36"/>
-      <c r="E57" s="36">
+      <c r="D57" s="37"/>
+      <c r="E57" s="37">
         <f t="shared" si="12"/>
         <v>5.4907810156274852</v>
       </c>
-      <c r="F57" s="36"/>
-      <c r="G57" s="25"/>
+      <c r="F57" s="37"/>
+      <c r="G57" s="51">
+        <f t="shared" si="13"/>
+        <v>388.72695253906875</v>
+      </c>
     </row>
     <row r="58" spans="1:29" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A58" s="30"/>
+      <c r="A58" s="28"/>
       <c r="B58" s="6">
         <v>4</v>
       </c>
-      <c r="C58" s="35">
+      <c r="C58" s="41">
         <f t="shared" si="11"/>
         <v>9.5832207228700061E-2</v>
       </c>
-      <c r="D58" s="36"/>
-      <c r="E58" s="36">
+      <c r="D58" s="37"/>
+      <c r="E58" s="37">
         <f t="shared" si="12"/>
         <v>5.4907810156276122</v>
       </c>
-      <c r="F58" s="36"/>
-      <c r="G58" s="25"/>
+      <c r="F58" s="37"/>
+      <c r="G58" s="51">
+        <f t="shared" si="13"/>
+        <v>388.72695253906903</v>
+      </c>
     </row>
     <row r="59" spans="1:29" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A59" s="30"/>
+      <c r="A59" s="28"/>
       <c r="B59" s="6">
         <v>5</v>
       </c>
-      <c r="C59" s="35">
+      <c r="C59" s="41">
         <f t="shared" si="11"/>
         <v>9.5832207228698674E-2</v>
       </c>
-      <c r="D59" s="36"/>
-      <c r="E59" s="36">
+      <c r="D59" s="37"/>
+      <c r="E59" s="37">
         <f t="shared" si="12"/>
         <v>5.4907810156275332</v>
       </c>
-      <c r="F59" s="36"/>
-      <c r="G59" s="25"/>
+      <c r="F59" s="37"/>
+      <c r="G59" s="51">
+        <f t="shared" si="13"/>
+        <v>388.72695253906886</v>
+      </c>
     </row>
     <row r="60" spans="1:29" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A60" s="31"/>
+      <c r="A60" s="29"/>
       <c r="B60" s="6">
         <v>6</v>
       </c>
-      <c r="C60" s="35">
+      <c r="C60" s="41">
         <f t="shared" si="11"/>
         <v>9.5832207228699173E-2</v>
       </c>
-      <c r="D60" s="36"/>
-      <c r="E60" s="36">
+      <c r="D60" s="37"/>
+      <c r="E60" s="37">
         <f t="shared" si="12"/>
         <v>5.4907810156275616</v>
       </c>
-      <c r="F60" s="36"/>
-      <c r="G60" s="25"/>
+      <c r="F60" s="37"/>
+      <c r="G60" s="51">
+        <f t="shared" si="13"/>
+        <v>388.72695253906892</v>
+      </c>
     </row>
     <row r="61" spans="1:29" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A61" s="20"/>
@@ -4559,9 +4734,25 @@
       <c r="E61" s="21"/>
       <c r="F61" s="22"/>
       <c r="G61" s="22"/>
+      <c r="J61" s="1"/>
+      <c r="K61" s="25" t="s">
+        <v>2</v>
+      </c>
+      <c r="L61" s="25" t="s">
+        <v>3</v>
+      </c>
+      <c r="M61" s="25" t="s">
+        <v>4</v>
+      </c>
+      <c r="N61" s="25" t="s">
+        <v>8</v>
+      </c>
+      <c r="O61" s="25" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="62" spans="1:29" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A62" s="26" t="s">
+      <c r="A62" s="43" t="s">
         <v>50</v>
       </c>
       <c r="B62" s="6">
@@ -4580,16 +4771,42 @@
         <v>3.8274236163370832</v>
       </c>
       <c r="F62" s="11">
-        <f t="shared" ref="F62:F77" si="13">(-0.35*C62)+D62</f>
+        <f t="shared" ref="F62:F77" si="14">(-0.35*C62)+D62</f>
         <v>158.83625015431414</v>
       </c>
       <c r="G62" s="11">
-        <f t="shared" ref="G62:G77" si="14">(-0.35*C62)+E62</f>
+        <f t="shared" ref="G62:G77" si="15">(-0.35*C62)+E62</f>
         <v>21.843710432906658</v>
       </c>
+      <c r="I62" s="27" t="s">
+        <v>51</v>
+      </c>
+      <c r="J62" s="25">
+        <v>1</v>
+      </c>
+      <c r="K62" s="11">
+        <f>C62</f>
+        <v>-51.475105190198789</v>
+      </c>
+      <c r="L62" s="11">
+        <f t="shared" ref="L62:O62" si="16">D62</f>
+        <v>140.81996333774458</v>
+      </c>
+      <c r="M62" s="11">
+        <f t="shared" si="16"/>
+        <v>3.8274236163370832</v>
+      </c>
+      <c r="N62" s="11">
+        <f t="shared" si="16"/>
+        <v>158.83625015431414</v>
+      </c>
+      <c r="O62" s="11">
+        <f t="shared" si="16"/>
+        <v>21.843710432906658</v>
+      </c>
     </row>
     <row r="63" spans="1:29" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A63" s="27"/>
+      <c r="A63" s="44"/>
       <c r="B63" s="6"/>
       <c r="C63" s="11">
         <f>C2</f>
@@ -4611,18 +4828,47 @@
         <f>G2</f>
         <v>5.9475624695284148</v>
       </c>
+      <c r="I63" s="28"/>
+      <c r="J63" s="25"/>
+      <c r="K63" s="11">
+        <f>C22</f>
+        <v>63.567076658305467</v>
+      </c>
+      <c r="L63" s="11">
+        <f t="shared" ref="L63:O63" si="17">D22</f>
+        <v>125.29755290953258</v>
+      </c>
+      <c r="M63" s="11">
+        <f t="shared" si="17"/>
+        <v>144</v>
+      </c>
+      <c r="N63" s="11">
+        <f t="shared" si="17"/>
+        <v>103.04907607912567</v>
+      </c>
+      <c r="O63" s="11">
+        <f t="shared" si="17"/>
+        <v>121.75152316959309</v>
+      </c>
     </row>
     <row r="64" spans="1:29" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A64" s="27"/>
+      <c r="A64" s="44"/>
       <c r="B64" s="6"/>
       <c r="C64" s="1"/>
       <c r="D64" s="1"/>
       <c r="E64" s="1"/>
       <c r="F64" s="11"/>
       <c r="G64" s="11"/>
-    </row>
-    <row r="65" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A65" s="27"/>
+      <c r="I64" s="28"/>
+      <c r="J64" s="25"/>
+      <c r="K64" s="11"/>
+      <c r="L64" s="11"/>
+      <c r="M64" s="11"/>
+      <c r="N64" s="11"/>
+      <c r="O64" s="11"/>
+    </row>
+    <row r="65" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A65" s="44"/>
       <c r="B65" s="6">
         <v>2</v>
       </c>
@@ -4639,16 +4885,40 @@
         <v>3.8274236163370654</v>
       </c>
       <c r="F65" s="11">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>148.66436998144388</v>
       </c>
       <c r="G65" s="11">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>37.503063171720314</v>
       </c>
-    </row>
-    <row r="66" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A66" s="27"/>
+      <c r="I65" s="28"/>
+      <c r="J65" s="25">
+        <v>2</v>
+      </c>
+      <c r="K65" s="11">
+        <f>C65</f>
+        <v>-96.216113015380728</v>
+      </c>
+      <c r="L65" s="11">
+        <f t="shared" ref="L65:O65" si="18">D65</f>
+        <v>114.98873042606063</v>
+      </c>
+      <c r="M65" s="11">
+        <f t="shared" si="18"/>
+        <v>3.8274236163370654</v>
+      </c>
+      <c r="N65" s="11">
+        <f t="shared" si="18"/>
+        <v>148.66436998144388</v>
+      </c>
+      <c r="O65" s="11">
+        <f t="shared" si="18"/>
+        <v>37.503063171720314</v>
+      </c>
+    </row>
+    <row r="66" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A66" s="44"/>
       <c r="B66" s="6"/>
       <c r="C66" s="11">
         <f>C3</f>
@@ -4670,18 +4940,47 @@
         <f>G3</f>
         <v>33.675639555383249</v>
       </c>
-    </row>
-    <row r="67" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A67" s="27"/>
+      <c r="I66" s="28"/>
+      <c r="J66" s="25"/>
+      <c r="K66" s="11">
+        <f>C23</f>
+        <v>-140.29440218083275</v>
+      </c>
+      <c r="L66" s="11">
+        <f t="shared" ref="L66:O66" si="19">D23</f>
+        <v>7.5980732243609284</v>
+      </c>
+      <c r="M66" s="11">
+        <f t="shared" si="19"/>
+        <v>144</v>
+      </c>
+      <c r="N66" s="11">
+        <f t="shared" si="19"/>
+        <v>56.701113987652391</v>
+      </c>
+      <c r="O66" s="11">
+        <f t="shared" si="19"/>
+        <v>193.10304076329146</v>
+      </c>
+    </row>
+    <row r="67" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A67" s="44"/>
       <c r="B67" s="6"/>
       <c r="C67" s="1"/>
       <c r="D67" s="1"/>
       <c r="E67" s="1"/>
       <c r="F67" s="11"/>
       <c r="G67" s="11"/>
-    </row>
-    <row r="68" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A68" s="27"/>
+      <c r="I67" s="28"/>
+      <c r="J67" s="25"/>
+      <c r="K67" s="11"/>
+      <c r="L67" s="11"/>
+      <c r="M67" s="11"/>
+      <c r="N67" s="11"/>
+      <c r="O67" s="11"/>
+    </row>
+    <row r="68" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A68" s="44"/>
       <c r="B68" s="6">
         <v>3</v>
       </c>
@@ -4698,16 +4997,40 @@
         <v>3.8274236163369943</v>
       </c>
       <c r="F68" s="11">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>-81.313090870677314</v>
       </c>
       <c r="G68" s="11">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>37.503063171720264</v>
       </c>
-    </row>
-    <row r="69" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A69" s="27"/>
+      <c r="I68" s="28"/>
+      <c r="J68" s="25">
+        <v>3</v>
+      </c>
+      <c r="K68" s="11">
+        <f>C68</f>
+        <v>-96.21611301538077</v>
+      </c>
+      <c r="L68" s="11">
+        <f t="shared" ref="L68:O68" si="20">D68</f>
+        <v>-114.98873042606058</v>
+      </c>
+      <c r="M68" s="11">
+        <f t="shared" si="20"/>
+        <v>3.8274236163369943</v>
+      </c>
+      <c r="N68" s="11">
+        <f t="shared" si="20"/>
+        <v>-81.313090870677314</v>
+      </c>
+      <c r="O68" s="11">
+        <f t="shared" si="20"/>
+        <v>37.503063171720264</v>
+      </c>
+    </row>
+    <row r="69" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A69" s="44"/>
       <c r="B69" s="6"/>
       <c r="C69" s="11">
         <f>C4</f>
@@ -4729,18 +5052,47 @@
         <f>G4</f>
         <v>33.67563955538327</v>
       </c>
-    </row>
-    <row r="70" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A70" s="27"/>
+      <c r="I69" s="28"/>
+      <c r="J69" s="25"/>
+      <c r="K69" s="11">
+        <f>C24</f>
+        <v>-140.29440218083275</v>
+      </c>
+      <c r="L69" s="11">
+        <f t="shared" ref="L69:O69" si="21">D24</f>
+        <v>-7.5980732243609808</v>
+      </c>
+      <c r="M69" s="11">
+        <f t="shared" si="21"/>
+        <v>144</v>
+      </c>
+      <c r="N69" s="11">
+        <f t="shared" si="21"/>
+        <v>41.50496753893048</v>
+      </c>
+      <c r="O69" s="11">
+        <f t="shared" si="21"/>
+        <v>193.10304076329146</v>
+      </c>
+    </row>
+    <row r="70" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A70" s="44"/>
       <c r="B70" s="6"/>
       <c r="C70" s="1"/>
       <c r="D70" s="1"/>
       <c r="E70" s="1"/>
       <c r="F70" s="11"/>
       <c r="G70" s="11"/>
-    </row>
-    <row r="71" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A71" s="27"/>
+      <c r="I70" s="28"/>
+      <c r="J70" s="25"/>
+      <c r="K70" s="11"/>
+      <c r="L70" s="11"/>
+      <c r="M70" s="11"/>
+      <c r="N70" s="11"/>
+      <c r="O70" s="11"/>
+    </row>
+    <row r="71" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A71" s="44"/>
       <c r="B71" s="6">
         <v>4</v>
       </c>
@@ -4757,16 +5109,40 @@
         <v>3.8274236163370832</v>
       </c>
       <c r="F71" s="11">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>-122.80367652117502</v>
       </c>
       <c r="G71" s="11">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>21.843710432906644</v>
       </c>
-    </row>
-    <row r="72" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A72" s="27"/>
+      <c r="I71" s="28"/>
+      <c r="J71" s="25">
+        <v>4</v>
+      </c>
+      <c r="K71" s="11">
+        <f>C71</f>
+        <v>-51.475105190198747</v>
+      </c>
+      <c r="L71" s="11">
+        <f t="shared" ref="L71:N71" si="22">D71</f>
+        <v>-140.81996333774458</v>
+      </c>
+      <c r="M71" s="11">
+        <f t="shared" si="22"/>
+        <v>3.8274236163370832</v>
+      </c>
+      <c r="N71" s="11">
+        <f t="shared" si="22"/>
+        <v>-122.80367652117502</v>
+      </c>
+      <c r="O71" s="11">
+        <f>G71</f>
+        <v>21.843710432906644</v>
+      </c>
+    </row>
+    <row r="72" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A72" s="44"/>
       <c r="B72" s="6"/>
       <c r="C72" s="11">
         <f>C5</f>
@@ -4788,18 +5164,47 @@
         <f>G5</f>
         <v>5.9475624695283997</v>
       </c>
-    </row>
-    <row r="73" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A73" s="27"/>
+      <c r="I72" s="28"/>
+      <c r="J72" s="25"/>
+      <c r="K72" s="11">
+        <f>C25</f>
+        <v>63.567076658305503</v>
+      </c>
+      <c r="L72" s="11">
+        <f t="shared" ref="L72:O72" si="23">D25</f>
+        <v>-125.29755290953256</v>
+      </c>
+      <c r="M72" s="11">
+        <f t="shared" si="23"/>
+        <v>144</v>
+      </c>
+      <c r="N72" s="11">
+        <f t="shared" si="23"/>
+        <v>-147.54602973993948</v>
+      </c>
+      <c r="O72" s="11">
+        <f t="shared" si="23"/>
+        <v>121.75152316959307</v>
+      </c>
+    </row>
+    <row r="73" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A73" s="44"/>
       <c r="B73" s="6"/>
       <c r="C73" s="1"/>
       <c r="D73" s="1"/>
       <c r="E73" s="1"/>
       <c r="F73" s="11"/>
       <c r="G73" s="11"/>
-    </row>
-    <row r="74" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A74" s="27"/>
+      <c r="I73" s="28"/>
+      <c r="J73" s="25"/>
+      <c r="K73" s="11"/>
+      <c r="L73" s="11"/>
+      <c r="M73" s="11"/>
+      <c r="N73" s="11"/>
+      <c r="O73" s="11"/>
+    </row>
+    <row r="74" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A74" s="44"/>
       <c r="B74" s="6">
         <v>5</v>
       </c>
@@ -4816,16 +5221,40 @@
         <v>3.8274236163370281</v>
       </c>
       <c r="F74" s="11">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>-77.523159283636829</v>
       </c>
       <c r="G74" s="11">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>-47.864502755615796</v>
       </c>
-    </row>
-    <row r="75" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A75" s="27"/>
+      <c r="I74" s="28"/>
+      <c r="J74" s="25">
+        <v>5</v>
+      </c>
+      <c r="K74" s="11">
+        <f>C74</f>
+        <v>147.6912182055795</v>
+      </c>
+      <c r="L74" s="11">
+        <f t="shared" ref="L74:O74" si="24">D74</f>
+        <v>-25.831232911683998</v>
+      </c>
+      <c r="M74" s="11">
+        <f t="shared" si="24"/>
+        <v>3.8274236163370281</v>
+      </c>
+      <c r="N74" s="11">
+        <f t="shared" si="24"/>
+        <v>-77.523159283636829</v>
+      </c>
+      <c r="O74" s="11">
+        <f t="shared" si="24"/>
+        <v>-47.864502755615796</v>
+      </c>
+    </row>
+    <row r="75" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A75" s="44"/>
       <c r="B75" s="6"/>
       <c r="C75" s="11">
         <f>C6</f>
@@ -4847,18 +5276,47 @@
         <f>G6</f>
         <v>-39.623202024911656</v>
       </c>
-    </row>
-    <row r="76" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A76" s="27"/>
+      <c r="I75" s="28"/>
+      <c r="J75" s="25"/>
+      <c r="K75" s="11">
+        <f>C26</f>
+        <v>76.727325522527309</v>
+      </c>
+      <c r="L75" s="11">
+        <f t="shared" ref="L75:O75" si="25">D26</f>
+        <v>-117.69947968517164</v>
+      </c>
+      <c r="M75" s="11">
+        <f t="shared" si="25"/>
+        <v>144</v>
+      </c>
+      <c r="N75" s="11">
+        <f t="shared" si="25"/>
+        <v>-144.5540436180562</v>
+      </c>
+      <c r="O75" s="11">
+        <f t="shared" si="25"/>
+        <v>117.14543606711544</v>
+      </c>
+    </row>
+    <row r="76" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A76" s="44"/>
       <c r="B76" s="6"/>
       <c r="C76" s="1"/>
       <c r="D76" s="1"/>
       <c r="E76" s="1"/>
       <c r="F76" s="11"/>
       <c r="G76" s="11"/>
-    </row>
-    <row r="77" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A77" s="27"/>
+      <c r="I76" s="28"/>
+      <c r="J76" s="25"/>
+      <c r="K76" s="11"/>
+      <c r="L76" s="11"/>
+      <c r="M76" s="11"/>
+      <c r="N76" s="11"/>
+      <c r="O76" s="11"/>
+    </row>
+    <row r="77" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A77" s="44"/>
       <c r="B77" s="6">
         <v>6</v>
       </c>
@@ -4875,16 +5333,40 @@
         <v>3.8274236163370476</v>
       </c>
       <c r="F77" s="11">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>-25.860693460268838</v>
       </c>
       <c r="G77" s="11">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>-47.864502755615774</v>
       </c>
-    </row>
-    <row r="78" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A78" s="28"/>
+      <c r="I77" s="28"/>
+      <c r="J77" s="25">
+        <v>6</v>
+      </c>
+      <c r="K77" s="11">
+        <f>C77</f>
+        <v>147.6912182055795</v>
+      </c>
+      <c r="L77" s="11">
+        <f t="shared" ref="L77:O77" si="26">D77</f>
+        <v>25.831232911683987</v>
+      </c>
+      <c r="M77" s="11">
+        <f t="shared" si="26"/>
+        <v>3.8274236163370476</v>
+      </c>
+      <c r="N77" s="11">
+        <f t="shared" si="26"/>
+        <v>-25.860693460268838</v>
+      </c>
+      <c r="O77" s="11">
+        <f t="shared" si="26"/>
+        <v>-47.864502755615774</v>
+      </c>
+    </row>
+    <row r="78" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A78" s="45"/>
       <c r="B78" s="2"/>
       <c r="C78" s="11">
         <f>C7</f>
@@ -4905,6 +5387,28 @@
       <c r="G78" s="11">
         <f>G7</f>
         <v>-39.623202024911656</v>
+      </c>
+      <c r="I78" s="29"/>
+      <c r="J78" s="25"/>
+      <c r="K78" s="11">
+        <f>C27</f>
+        <v>76.727325522527281</v>
+      </c>
+      <c r="L78" s="11">
+        <f t="shared" ref="L78:O78" si="27">D27</f>
+        <v>117.69947968517164</v>
+      </c>
+      <c r="M78" s="11">
+        <f t="shared" si="27"/>
+        <v>144</v>
+      </c>
+      <c r="N78" s="11">
+        <f t="shared" si="27"/>
+        <v>90.844915752287093</v>
+      </c>
+      <c r="O78" s="11">
+        <f t="shared" si="27"/>
+        <v>117.14543606711545</v>
       </c>
     </row>
     <row r="84" spans="6:7" x14ac:dyDescent="0.3">
@@ -4995,30 +5499,8 @@
       <c r="G114" s="17"/>
     </row>
   </sheetData>
-  <mergeCells count="39">
-    <mergeCell ref="A10:A20"/>
-    <mergeCell ref="A22:A28"/>
-    <mergeCell ref="A2:A8"/>
-    <mergeCell ref="W8:AC8"/>
-    <mergeCell ref="T24:U24"/>
-    <mergeCell ref="T20:U20"/>
-    <mergeCell ref="T8:U8"/>
-    <mergeCell ref="T2:U2"/>
-    <mergeCell ref="E60:F60"/>
-    <mergeCell ref="Z20:AB20"/>
-    <mergeCell ref="W2:Y2"/>
-    <mergeCell ref="W20:X20"/>
-    <mergeCell ref="W21:X21"/>
-    <mergeCell ref="W22:X22"/>
-    <mergeCell ref="W23:X23"/>
-    <mergeCell ref="T31:T36"/>
-    <mergeCell ref="T37:T42"/>
-    <mergeCell ref="T43:T48"/>
-    <mergeCell ref="E55:F55"/>
-    <mergeCell ref="E56:F56"/>
-    <mergeCell ref="E57:F57"/>
-    <mergeCell ref="E58:F58"/>
-    <mergeCell ref="E59:F59"/>
+  <mergeCells count="40">
+    <mergeCell ref="I62:I78"/>
     <mergeCell ref="A62:A78"/>
     <mergeCell ref="A37:A53"/>
     <mergeCell ref="A30:A35"/>
@@ -5035,6 +5517,29 @@
     <mergeCell ref="C59:D59"/>
     <mergeCell ref="C60:D60"/>
     <mergeCell ref="A55:A60"/>
+    <mergeCell ref="E60:F60"/>
+    <mergeCell ref="Z20:AB20"/>
+    <mergeCell ref="W2:Y2"/>
+    <mergeCell ref="W20:X20"/>
+    <mergeCell ref="W21:X21"/>
+    <mergeCell ref="W22:X22"/>
+    <mergeCell ref="W23:X23"/>
+    <mergeCell ref="T31:T36"/>
+    <mergeCell ref="T37:T42"/>
+    <mergeCell ref="T43:T48"/>
+    <mergeCell ref="E55:F55"/>
+    <mergeCell ref="E56:F56"/>
+    <mergeCell ref="E57:F57"/>
+    <mergeCell ref="E58:F58"/>
+    <mergeCell ref="E59:F59"/>
+    <mergeCell ref="A10:A20"/>
+    <mergeCell ref="A22:A28"/>
+    <mergeCell ref="A2:A8"/>
+    <mergeCell ref="W8:AC8"/>
+    <mergeCell ref="T24:U24"/>
+    <mergeCell ref="T20:U20"/>
+    <mergeCell ref="T8:U8"/>
+    <mergeCell ref="T2:U2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>

<commit_message>
Overhauled mathematics and logic. SIM WORKS
</commit_message>
<xml_diff>
--- a/Sim_Emulator.xlsx
+++ b/Sim_Emulator.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
-  <workbookPr codeName="ThisWorkbook"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22325"/>
+  <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MiniSim\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86B46CBE-1461-4707-86EB-6983FE6BD546}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38280" yWindow="-120" windowWidth="38640" windowHeight="21240"/>
+    <workbookView xWindow="43080" yWindow="4680" windowWidth="28800" windowHeight="15435" tabRatio="193" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -22,15 +23,39 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
+<file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+  <metadataTypes count="1">
+    <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
+  </metadataTypes>
+  <futureMetadata name="XLDAPR" count="1">
+    <bk>
+      <extLst>
+        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
+          <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
+        </ext>
+      </extLst>
+    </bk>
+  </futureMetadata>
+  <cellMetadata count="1">
+    <bk>
+      <rc t="1" v="0"/>
+    </bk>
+  </cellMetadata>
+</metadata>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="56">
   <si>
     <t>Translational</t>
   </si>
@@ -203,11 +228,11 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="7">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -378,7 +403,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="52">
+  <cellXfs count="53">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -438,6 +463,16 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -510,13 +545,6 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1280,7 +1308,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1312,7 +1339,6 @@
     </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
-    <c:showDLblsOverMax val="0"/>
     <c:extLst>
       <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
         <c16r3:dataDisplayOptions16>
@@ -1320,6 +1346,7 @@
         </c16r3:dataDisplayOptions16>
       </c:ext>
     </c:extLst>
+    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
     <a:solidFill>
@@ -1911,51 +1938,27 @@
 </file>
 
 <file path=xl/ctrlProps/ctrlProp1.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Scroll" dx="22" fmlaLink="$X$49" max="100" page="0" val="50"/>
-</file>
-
-<file path=xl/ctrlProps/ctrlProp10.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Spin" dx="26" fmlaLink="$AC$49" max="90" noThreeD="1" page="10" val="45"/>
-</file>
-
-<file path=xl/ctrlProps/ctrlProp11.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Spin" dx="26" fmlaLink="$Y$49" max="100" noThreeD="1" page="10" val="50"/>
-</file>
-
-<file path=xl/ctrlProps/ctrlProp12.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Spin" dx="26" fmlaLink="$X$49" max="100" noThreeD="1" page="10" val="50"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Spin" dx="26" fmlaLink="$Z$29" max="100" noThreeD="1" page="10" val="50"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp2.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Scroll" dx="22" fmlaLink="$Y$49" max="100" page="0" val="50"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Spin" dx="26" fmlaLink="$AA$29" max="90" noThreeD="1" page="10" val="45"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp3.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Scroll" dx="22" fmlaLink="$Z$49" max="100" page="0" val="50"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Spin" dx="26" fmlaLink="AB$29" max="90" noThreeD="1" page="10" val="45"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp4.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Scroll" dx="22" fmlaLink="$AA$49" max="90" page="0" val="45"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Spin" dx="26" fmlaLink="$AC$29" max="90" noThreeD="1" page="10" val="45"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp5.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Scroll" dx="22" fmlaLink="$AB$49" max="90" page="0" val="45"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Spin" dx="26" fmlaLink="$Y$29" max="100" noThreeD="1" page="10" val="50"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp6.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Scroll" dx="22" fmlaLink="$AC$49" max="90" page="0" val="45"/>
-</file>
-
-<file path=xl/ctrlProps/ctrlProp7.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Spin" dx="26" fmlaLink="$Z$49" max="100" noThreeD="1" page="10" val="50"/>
-</file>
-
-<file path=xl/ctrlProps/ctrlProp8.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Spin" dx="26" fmlaLink="$AA$49" max="90" noThreeD="1" page="10" val="45"/>
-</file>
-
-<file path=xl/ctrlProps/ctrlProp9.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Spin" dx="26" fmlaLink="AB$49" max="90" noThreeD="1" page="10" val="45"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Spin" dx="26" fmlaLink="$X$29" max="100" noThreeD="1" page="10" val="50"/>
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1978,7 +1981,7 @@
         <xdr:cNvPr id="3" name="Chart 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D3249A7C-5804-426C-AD8F-11820261C737}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000003000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1998,318 +2001,18 @@
   </xdr:twoCellAnchor>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
-      <xdr:twoCellAnchor editAs="oneCell">
-        <xdr:from>
-          <xdr:col>23</xdr:col>
-          <xdr:colOff>83820</xdr:colOff>
-          <xdr:row>28</xdr:row>
-          <xdr:rowOff>0</xdr:rowOff>
-        </xdr:from>
-        <xdr:to>
-          <xdr:col>23</xdr:col>
-          <xdr:colOff>556260</xdr:colOff>
-          <xdr:row>45</xdr:row>
-          <xdr:rowOff>106680</xdr:rowOff>
-        </xdr:to>
-        <xdr:sp macro="" textlink="">
-          <xdr:nvSpPr>
-            <xdr:cNvPr id="1038" name="Scroll Bar 14" hidden="1">
-              <a:extLst>
-                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
-                  <a14:compatExt spid="_x0000_s1038"/>
-                </a:ext>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5FA9FC04-E975-4443-8097-1443486CB6EC}"/>
-                </a:ext>
-              </a:extLst>
-            </xdr:cNvPr>
-            <xdr:cNvSpPr/>
-          </xdr:nvSpPr>
-          <xdr:spPr bwMode="auto">
-            <a:xfrm>
-              <a:off x="0" y="0"/>
-              <a:ext cx="0" cy="0"/>
-            </a:xfrm>
-            <a:prstGeom prst="rect">
-              <a:avLst/>
-            </a:prstGeom>
-            <a:noFill/>
-            <a:ln w="9525">
-              <a:miter lim="800000"/>
-              <a:headEnd/>
-              <a:tailEnd/>
-            </a:ln>
-          </xdr:spPr>
-        </xdr:sp>
-        <xdr:clientData/>
-      </xdr:twoCellAnchor>
-    </mc:Choice>
-    <mc:Fallback/>
-  </mc:AlternateContent>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
-      <xdr:twoCellAnchor editAs="oneCell">
-        <xdr:from>
-          <xdr:col>24</xdr:col>
-          <xdr:colOff>76200</xdr:colOff>
-          <xdr:row>27</xdr:row>
-          <xdr:rowOff>190500</xdr:rowOff>
-        </xdr:from>
-        <xdr:to>
-          <xdr:col>24</xdr:col>
-          <xdr:colOff>525780</xdr:colOff>
-          <xdr:row>45</xdr:row>
-          <xdr:rowOff>99060</xdr:rowOff>
-        </xdr:to>
-        <xdr:sp macro="" textlink="">
-          <xdr:nvSpPr>
-            <xdr:cNvPr id="1039" name="Scroll Bar 15" hidden="1">
-              <a:extLst>
-                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
-                  <a14:compatExt spid="_x0000_s1039"/>
-                </a:ext>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{08DA8E45-DF6E-42C5-966D-DB475728E4A1}"/>
-                </a:ext>
-              </a:extLst>
-            </xdr:cNvPr>
-            <xdr:cNvSpPr/>
-          </xdr:nvSpPr>
-          <xdr:spPr bwMode="auto">
-            <a:xfrm>
-              <a:off x="0" y="0"/>
-              <a:ext cx="0" cy="0"/>
-            </a:xfrm>
-            <a:prstGeom prst="rect">
-              <a:avLst/>
-            </a:prstGeom>
-            <a:noFill/>
-            <a:ln w="9525">
-              <a:miter lim="800000"/>
-              <a:headEnd/>
-              <a:tailEnd/>
-            </a:ln>
-          </xdr:spPr>
-        </xdr:sp>
-        <xdr:clientData/>
-      </xdr:twoCellAnchor>
-    </mc:Choice>
-    <mc:Fallback/>
-  </mc:AlternateContent>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
-      <xdr:twoCellAnchor editAs="oneCell">
+      <xdr:twoCellAnchor>
         <xdr:from>
           <xdr:col>25</xdr:col>
-          <xdr:colOff>83820</xdr:colOff>
-          <xdr:row>28</xdr:row>
-          <xdr:rowOff>0</xdr:rowOff>
+          <xdr:colOff>47625</xdr:colOff>
+          <xdr:row>29</xdr:row>
+          <xdr:rowOff>47625</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>25</xdr:col>
-          <xdr:colOff>541020</xdr:colOff>
-          <xdr:row>45</xdr:row>
-          <xdr:rowOff>99060</xdr:rowOff>
-        </xdr:to>
-        <xdr:sp macro="" textlink="">
-          <xdr:nvSpPr>
-            <xdr:cNvPr id="1040" name="Scroll Bar 16" hidden="1">
-              <a:extLst>
-                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
-                  <a14:compatExt spid="_x0000_s1040"/>
-                </a:ext>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0D41FC32-E806-4BC5-BDC7-B018E35B6B46}"/>
-                </a:ext>
-              </a:extLst>
-            </xdr:cNvPr>
-            <xdr:cNvSpPr/>
-          </xdr:nvSpPr>
-          <xdr:spPr bwMode="auto">
-            <a:xfrm>
-              <a:off x="0" y="0"/>
-              <a:ext cx="0" cy="0"/>
-            </a:xfrm>
-            <a:prstGeom prst="rect">
-              <a:avLst/>
-            </a:prstGeom>
-            <a:noFill/>
-            <a:ln w="9525">
-              <a:miter lim="800000"/>
-              <a:headEnd/>
-              <a:tailEnd/>
-            </a:ln>
-          </xdr:spPr>
-        </xdr:sp>
-        <xdr:clientData/>
-      </xdr:twoCellAnchor>
-    </mc:Choice>
-    <mc:Fallback/>
-  </mc:AlternateContent>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
-      <xdr:twoCellAnchor editAs="oneCell">
-        <xdr:from>
-          <xdr:col>26</xdr:col>
-          <xdr:colOff>83820</xdr:colOff>
-          <xdr:row>28</xdr:row>
-          <xdr:rowOff>0</xdr:rowOff>
-        </xdr:from>
-        <xdr:to>
-          <xdr:col>26</xdr:col>
-          <xdr:colOff>533400</xdr:colOff>
-          <xdr:row>45</xdr:row>
-          <xdr:rowOff>99060</xdr:rowOff>
-        </xdr:to>
-        <xdr:sp macro="" textlink="">
-          <xdr:nvSpPr>
-            <xdr:cNvPr id="1041" name="Scroll Bar 17" hidden="1">
-              <a:extLst>
-                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
-                  <a14:compatExt spid="_x0000_s1041"/>
-                </a:ext>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1FAFFFF8-4822-4685-8622-9B4615764CDD}"/>
-                </a:ext>
-              </a:extLst>
-            </xdr:cNvPr>
-            <xdr:cNvSpPr/>
-          </xdr:nvSpPr>
-          <xdr:spPr bwMode="auto">
-            <a:xfrm>
-              <a:off x="0" y="0"/>
-              <a:ext cx="0" cy="0"/>
-            </a:xfrm>
-            <a:prstGeom prst="rect">
-              <a:avLst/>
-            </a:prstGeom>
-            <a:noFill/>
-            <a:ln w="9525">
-              <a:miter lim="800000"/>
-              <a:headEnd/>
-              <a:tailEnd/>
-            </a:ln>
-          </xdr:spPr>
-        </xdr:sp>
-        <xdr:clientData/>
-      </xdr:twoCellAnchor>
-    </mc:Choice>
-    <mc:Fallback/>
-  </mc:AlternateContent>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
-      <xdr:twoCellAnchor editAs="oneCell">
-        <xdr:from>
-          <xdr:col>27</xdr:col>
-          <xdr:colOff>68580</xdr:colOff>
-          <xdr:row>27</xdr:row>
-          <xdr:rowOff>190500</xdr:rowOff>
-        </xdr:from>
-        <xdr:to>
-          <xdr:col>27</xdr:col>
-          <xdr:colOff>525780</xdr:colOff>
-          <xdr:row>45</xdr:row>
-          <xdr:rowOff>99060</xdr:rowOff>
-        </xdr:to>
-        <xdr:sp macro="" textlink="">
-          <xdr:nvSpPr>
-            <xdr:cNvPr id="1042" name="Scroll Bar 18" hidden="1">
-              <a:extLst>
-                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
-                  <a14:compatExt spid="_x0000_s1042"/>
-                </a:ext>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{89F92E88-EA70-4353-A978-EE40A0380767}"/>
-                </a:ext>
-              </a:extLst>
-            </xdr:cNvPr>
-            <xdr:cNvSpPr/>
-          </xdr:nvSpPr>
-          <xdr:spPr bwMode="auto">
-            <a:xfrm>
-              <a:off x="0" y="0"/>
-              <a:ext cx="0" cy="0"/>
-            </a:xfrm>
-            <a:prstGeom prst="rect">
-              <a:avLst/>
-            </a:prstGeom>
-            <a:noFill/>
-            <a:ln w="9525">
-              <a:miter lim="800000"/>
-              <a:headEnd/>
-              <a:tailEnd/>
-            </a:ln>
-          </xdr:spPr>
-        </xdr:sp>
-        <xdr:clientData/>
-      </xdr:twoCellAnchor>
-    </mc:Choice>
-    <mc:Fallback/>
-  </mc:AlternateContent>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
-      <xdr:twoCellAnchor editAs="oneCell">
-        <xdr:from>
-          <xdr:col>28</xdr:col>
-          <xdr:colOff>60960</xdr:colOff>
-          <xdr:row>28</xdr:row>
-          <xdr:rowOff>0</xdr:rowOff>
-        </xdr:from>
-        <xdr:to>
-          <xdr:col>28</xdr:col>
-          <xdr:colOff>518160</xdr:colOff>
-          <xdr:row>45</xdr:row>
-          <xdr:rowOff>99060</xdr:rowOff>
-        </xdr:to>
-        <xdr:sp macro="" textlink="">
-          <xdr:nvSpPr>
-            <xdr:cNvPr id="1043" name="Scroll Bar 19" hidden="1">
-              <a:extLst>
-                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
-                  <a14:compatExt spid="_x0000_s1043"/>
-                </a:ext>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E154ADE3-A4FC-4F1C-833D-FBA8C81DE9A1}"/>
-                </a:ext>
-              </a:extLst>
-            </xdr:cNvPr>
-            <xdr:cNvSpPr/>
-          </xdr:nvSpPr>
-          <xdr:spPr bwMode="auto">
-            <a:xfrm>
-              <a:off x="0" y="0"/>
-              <a:ext cx="0" cy="0"/>
-            </a:xfrm>
-            <a:prstGeom prst="rect">
-              <a:avLst/>
-            </a:prstGeom>
-            <a:noFill/>
-            <a:ln w="9525">
-              <a:miter lim="800000"/>
-              <a:headEnd/>
-              <a:tailEnd/>
-            </a:ln>
-          </xdr:spPr>
-        </xdr:sp>
-        <xdr:clientData/>
-      </xdr:twoCellAnchor>
-    </mc:Choice>
-    <mc:Fallback/>
-  </mc:AlternateContent>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
-      <xdr:twoCellAnchor>
-        <xdr:from>
-          <xdr:col>25</xdr:col>
-          <xdr:colOff>60960</xdr:colOff>
-          <xdr:row>49</xdr:row>
-          <xdr:rowOff>190500</xdr:rowOff>
-        </xdr:from>
-        <xdr:to>
-          <xdr:col>25</xdr:col>
-          <xdr:colOff>548640</xdr:colOff>
-          <xdr:row>57</xdr:row>
-          <xdr:rowOff>22860</xdr:rowOff>
+          <xdr:colOff>542925</xdr:colOff>
+          <xdr:row>36</xdr:row>
+          <xdr:rowOff>66675</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -2317,6 +2020,9 @@
               <a:extLst>
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
                   <a14:compatExt spid="_x0000_s1044"/>
+                </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000014040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -2348,15 +2054,15 @@
       <xdr:twoCellAnchor>
         <xdr:from>
           <xdr:col>26</xdr:col>
-          <xdr:colOff>76200</xdr:colOff>
-          <xdr:row>50</xdr:row>
-          <xdr:rowOff>0</xdr:rowOff>
+          <xdr:colOff>66675</xdr:colOff>
+          <xdr:row>29</xdr:row>
+          <xdr:rowOff>47625</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>26</xdr:col>
-          <xdr:colOff>563880</xdr:colOff>
-          <xdr:row>57</xdr:row>
-          <xdr:rowOff>30480</xdr:rowOff>
+          <xdr:colOff>552450</xdr:colOff>
+          <xdr:row>36</xdr:row>
+          <xdr:rowOff>76200</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -2364,6 +2070,9 @@
               <a:extLst>
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
                   <a14:compatExt spid="_x0000_s1046"/>
+                </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000016040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -2395,15 +2104,15 @@
       <xdr:twoCellAnchor>
         <xdr:from>
           <xdr:col>27</xdr:col>
-          <xdr:colOff>68580</xdr:colOff>
-          <xdr:row>49</xdr:row>
-          <xdr:rowOff>190500</xdr:rowOff>
+          <xdr:colOff>57150</xdr:colOff>
+          <xdr:row>29</xdr:row>
+          <xdr:rowOff>47625</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>27</xdr:col>
-          <xdr:colOff>548640</xdr:colOff>
-          <xdr:row>57</xdr:row>
-          <xdr:rowOff>22860</xdr:rowOff>
+          <xdr:colOff>542925</xdr:colOff>
+          <xdr:row>36</xdr:row>
+          <xdr:rowOff>66675</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -2411,6 +2120,9 @@
               <a:extLst>
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
                   <a14:compatExt spid="_x0000_s1047"/>
+                </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000017040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -2442,15 +2154,15 @@
       <xdr:twoCellAnchor>
         <xdr:from>
           <xdr:col>28</xdr:col>
-          <xdr:colOff>60960</xdr:colOff>
-          <xdr:row>50</xdr:row>
-          <xdr:rowOff>0</xdr:rowOff>
+          <xdr:colOff>47625</xdr:colOff>
+          <xdr:row>29</xdr:row>
+          <xdr:rowOff>47625</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>28</xdr:col>
-          <xdr:colOff>541020</xdr:colOff>
-          <xdr:row>57</xdr:row>
-          <xdr:rowOff>22860</xdr:rowOff>
+          <xdr:colOff>533400</xdr:colOff>
+          <xdr:row>36</xdr:row>
+          <xdr:rowOff>66675</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -2458,6 +2170,9 @@
               <a:extLst>
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
                   <a14:compatExt spid="_x0000_s1048"/>
+                </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000018040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -2489,15 +2204,15 @@
       <xdr:twoCellAnchor>
         <xdr:from>
           <xdr:col>24</xdr:col>
-          <xdr:colOff>76200</xdr:colOff>
-          <xdr:row>49</xdr:row>
-          <xdr:rowOff>190500</xdr:rowOff>
+          <xdr:colOff>66675</xdr:colOff>
+          <xdr:row>29</xdr:row>
+          <xdr:rowOff>47625</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>24</xdr:col>
-          <xdr:colOff>556260</xdr:colOff>
-          <xdr:row>57</xdr:row>
-          <xdr:rowOff>22860</xdr:rowOff>
+          <xdr:colOff>542925</xdr:colOff>
+          <xdr:row>36</xdr:row>
+          <xdr:rowOff>66675</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -2505,6 +2220,9 @@
               <a:extLst>
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
                   <a14:compatExt spid="_x0000_s1049"/>
+                </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000019040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -2536,15 +2254,15 @@
       <xdr:twoCellAnchor>
         <xdr:from>
           <xdr:col>23</xdr:col>
-          <xdr:colOff>91440</xdr:colOff>
-          <xdr:row>50</xdr:row>
-          <xdr:rowOff>0</xdr:rowOff>
+          <xdr:colOff>85725</xdr:colOff>
+          <xdr:row>29</xdr:row>
+          <xdr:rowOff>47625</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>23</xdr:col>
-          <xdr:colOff>571500</xdr:colOff>
-          <xdr:row>57</xdr:row>
-          <xdr:rowOff>22860</xdr:rowOff>
+          <xdr:colOff>561975</xdr:colOff>
+          <xdr:row>36</xdr:row>
+          <xdr:rowOff>66675</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -2552,6 +2270,9 @@
               <a:extLst>
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
                   <a14:compatExt spid="_x0000_s1050"/>
+                </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00001A040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -2877,32 +2598,33 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:AC114"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="54" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="L57" sqref="L57"/>
+    <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+      <selection activeCell="H55" sqref="H55"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="18.6640625" customWidth="1"/>
+    <col min="1" max="1" width="18.7109375" customWidth="1"/>
     <col min="4" max="4" width="9" customWidth="1"/>
-    <col min="8" max="8" width="10.109375" customWidth="1"/>
+    <col min="7" max="7" width="11.7109375" customWidth="1"/>
+    <col min="8" max="8" width="10.140625" customWidth="1"/>
     <col min="9" max="9" width="22" customWidth="1"/>
-    <col min="10" max="11" width="10.6640625" customWidth="1"/>
-    <col min="12" max="12" width="11.6640625" customWidth="1"/>
-    <col min="13" max="15" width="10.6640625" customWidth="1"/>
-    <col min="17" max="17" width="20.44140625" customWidth="1"/>
-    <col min="18" max="19" width="11.5546875" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="12.6640625" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="11.5546875" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="14.33203125" customWidth="1"/>
+    <col min="10" max="11" width="10.7109375" customWidth="1"/>
+    <col min="12" max="12" width="11.7109375" customWidth="1"/>
+    <col min="13" max="15" width="10.7109375" customWidth="1"/>
+    <col min="17" max="17" width="20.42578125" customWidth="1"/>
+    <col min="18" max="19" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="14.28515625" customWidth="1"/>
     <col min="23" max="23" width="21" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:29">
       <c r="A1" s="1"/>
       <c r="B1" s="1"/>
       <c r="C1" s="6" t="s">
@@ -2921,8 +2643,8 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:29" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="27" t="s">
+    <row r="2" spans="1:29" ht="15" customHeight="1">
+      <c r="A2" s="31" t="s">
         <v>7</v>
       </c>
       <c r="B2" s="6">
@@ -2947,18 +2669,18 @@
         <f t="shared" ref="G2:G7" si="1">(-0.35*C2)+E2</f>
         <v>5.9475624695284148</v>
       </c>
-      <c r="T2" s="35" t="s">
+      <c r="T2" s="39" t="s">
         <v>12</v>
       </c>
-      <c r="U2" s="36"/>
-      <c r="W2" s="35" t="s">
+      <c r="U2" s="40"/>
+      <c r="W2" s="39" t="s">
         <v>13</v>
       </c>
-      <c r="X2" s="38"/>
-      <c r="Y2" s="36"/>
-    </row>
-    <row r="3" spans="1:29" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="28"/>
+      <c r="X2" s="42"/>
+      <c r="Y2" s="40"/>
+    </row>
+    <row r="3" spans="1:29" ht="15" customHeight="1">
+      <c r="A3" s="32"/>
       <c r="B3" s="6">
         <v>2</v>
       </c>
@@ -2985,14 +2707,14 @@
         <v>17</v>
       </c>
       <c r="U3" s="10">
-        <f>((X49-0)*(50+50))/(100-0)-50</f>
+        <f>((X29-0)*(50+50))/(100-0)-50</f>
         <v>0</v>
       </c>
       <c r="W3" s="7" t="s">
         <v>14</v>
       </c>
       <c r="X3" s="5">
-        <f>((AA49-0)*(45+45))/(90-0)-45</f>
+        <f>((AA29-0)*(45+45))/(90-0)-45</f>
         <v>0</v>
       </c>
       <c r="Y3" s="5">
@@ -3000,8 +2722,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:29" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="28"/>
+    <row r="4" spans="1:29" ht="15" customHeight="1">
+      <c r="A4" s="32"/>
       <c r="B4" s="6">
         <v>3</v>
       </c>
@@ -3028,14 +2750,14 @@
         <v>18</v>
       </c>
       <c r="U4" s="10">
-        <f>((Y49-0)*(50+50))/(100-0)-50</f>
+        <f>((Y29-0)*(50+50))/(100-0)-50</f>
         <v>0</v>
       </c>
       <c r="W4" s="7" t="s">
         <v>15</v>
       </c>
       <c r="X4" s="5">
-        <f>((AB49-0)*(45+45))/(90-0)-45</f>
+        <f>((AB29-0)*(45+45))/(90-0)-45</f>
         <v>0</v>
       </c>
       <c r="Y4" s="5">
@@ -3043,8 +2765,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:29" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="28"/>
+    <row r="5" spans="1:29" ht="15" customHeight="1">
+      <c r="A5" s="32"/>
       <c r="B5" s="6">
         <v>4</v>
       </c>
@@ -3071,14 +2793,14 @@
         <v>19</v>
       </c>
       <c r="U5" s="10">
-        <f>((Z49-0)*(50+50))/(100-0)-50</f>
+        <f>((Z29-0)*(50+50))/(100-0)-50</f>
         <v>0</v>
       </c>
       <c r="W5" s="7" t="s">
         <v>16</v>
       </c>
       <c r="X5" s="5">
-        <f>((AC49-0)*(45+45))/(90-0)-45</f>
+        <f>((AC29-0)*(45+45))/(90-0)-45</f>
         <v>0</v>
       </c>
       <c r="Y5" s="5">
@@ -3086,8 +2808,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:29" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="28"/>
+    <row r="6" spans="1:29" ht="15" customHeight="1">
+      <c r="A6" s="32"/>
       <c r="B6" s="6">
         <v>5</v>
       </c>
@@ -3111,8 +2833,8 @@
         <v>-39.623202024911656</v>
       </c>
     </row>
-    <row r="7" spans="1:29" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="28"/>
+    <row r="7" spans="1:29" ht="15" customHeight="1">
+      <c r="A7" s="32"/>
       <c r="B7" s="6">
         <v>6</v>
       </c>
@@ -3136,8 +2858,8 @@
         <v>-39.623202024911656</v>
       </c>
     </row>
-    <row r="8" spans="1:29" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="29"/>
+    <row r="8" spans="1:29" ht="15" customHeight="1">
+      <c r="A8" s="33"/>
       <c r="B8" s="6" t="s">
         <v>39</v>
       </c>
@@ -3152,21 +2874,21 @@
         <f>(-0.35*C2)+E2</f>
         <v>5.9475624695284148</v>
       </c>
-      <c r="T8" s="35" t="s">
+      <c r="T8" s="39" t="s">
         <v>24</v>
       </c>
-      <c r="U8" s="36"/>
-      <c r="W8" s="30" t="s">
+      <c r="U8" s="40"/>
+      <c r="W8" s="34" t="s">
         <v>35</v>
       </c>
-      <c r="X8" s="31"/>
-      <c r="Y8" s="31"/>
-      <c r="Z8" s="31"/>
-      <c r="AA8" s="31"/>
-      <c r="AB8" s="31"/>
-      <c r="AC8" s="32"/>
-    </row>
-    <row r="9" spans="1:29" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="X8" s="35"/>
+      <c r="Y8" s="35"/>
+      <c r="Z8" s="35"/>
+      <c r="AA8" s="35"/>
+      <c r="AB8" s="35"/>
+      <c r="AC8" s="36"/>
+    </row>
+    <row r="9" spans="1:29" ht="15" customHeight="1">
       <c r="A9" s="20"/>
       <c r="B9" s="20"/>
       <c r="C9" s="21"/>
@@ -3200,8 +2922,8 @@
         <v>6</v>
       </c>
     </row>
-    <row r="10" spans="1:29" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="26" t="s">
+    <row r="10" spans="1:29" ht="15" customHeight="1">
+      <c r="A10" s="30" t="s">
         <v>10</v>
       </c>
       <c r="B10" s="6">
@@ -3254,8 +2976,8 @@
         <v>68</v>
       </c>
     </row>
-    <row r="11" spans="1:29" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="26"/>
+    <row r="11" spans="1:29" ht="15" customHeight="1">
+      <c r="A11" s="30"/>
       <c r="B11" s="6"/>
       <c r="C11" s="11"/>
       <c r="D11" s="11"/>
@@ -3296,8 +3018,8 @@
         <v>1.1868238913561442</v>
       </c>
     </row>
-    <row r="12" spans="1:29" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="26"/>
+    <row r="12" spans="1:29" ht="15" customHeight="1">
+      <c r="A12" s="30"/>
       <c r="B12" s="6">
         <v>2</v>
       </c>
@@ -3354,8 +3076,8 @@
         <v>122.1</v>
       </c>
     </row>
-    <row r="13" spans="1:29" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="26"/>
+    <row r="13" spans="1:29" ht="15" customHeight="1">
+      <c r="A13" s="30"/>
       <c r="B13" s="6"/>
       <c r="C13" s="11"/>
       <c r="D13" s="11"/>
@@ -3390,8 +3112,8 @@
         <v>33.1</v>
       </c>
     </row>
-    <row r="14" spans="1:29" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="26"/>
+    <row r="14" spans="1:29" ht="15" customHeight="1">
+      <c r="A14" s="30"/>
       <c r="B14" s="6">
         <v>3</v>
       </c>
@@ -3448,8 +3170,8 @@
         <v>0.57770398241012311</v>
       </c>
     </row>
-    <row r="15" spans="1:29" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="26"/>
+    <row r="15" spans="1:29" ht="15" customHeight="1">
+      <c r="A15" s="30"/>
       <c r="B15" s="6"/>
       <c r="C15" s="11"/>
       <c r="D15" s="11"/>
@@ -3490,8 +3212,8 @@
         <v>140.5</v>
       </c>
     </row>
-    <row r="16" spans="1:29" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="26"/>
+    <row r="16" spans="1:29" ht="15" customHeight="1">
+      <c r="A16" s="30"/>
       <c r="B16" s="6">
         <v>4</v>
       </c>
@@ -3542,8 +3264,8 @@
         <v>-30</v>
       </c>
     </row>
-    <row r="17" spans="1:29" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="26"/>
+    <row r="17" spans="1:29" ht="15" customHeight="1">
+      <c r="A17" s="30"/>
       <c r="B17" s="6"/>
       <c r="C17" s="11"/>
       <c r="D17" s="11"/>
@@ -3584,8 +3306,8 @@
         <v>-0.52359877559829882</v>
       </c>
     </row>
-    <row r="18" spans="1:29" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="26"/>
+    <row r="18" spans="1:29" ht="15" customHeight="1">
+      <c r="A18" s="30"/>
       <c r="B18" s="6">
         <v>5</v>
       </c>
@@ -3608,30 +3330,30 @@
         <f>(-0.35*C18)+E18</f>
         <v>-26.854563932884556</v>
       </c>
-      <c r="T18" s="49" t="s">
+      <c r="T18" s="26" t="s">
         <v>54</v>
       </c>
-      <c r="U18" s="50">
+      <c r="U18" s="27">
         <v>-90</v>
       </c>
     </row>
-    <row r="19" spans="1:29" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="26"/>
+    <row r="19" spans="1:29" ht="15" customHeight="1">
+      <c r="A19" s="30"/>
       <c r="B19" s="6"/>
       <c r="C19" s="11"/>
       <c r="D19" s="11"/>
       <c r="E19" s="11"/>
       <c r="F19" s="11"/>
       <c r="G19" s="11"/>
-      <c r="T19" s="49" t="s">
+      <c r="T19" s="26" t="s">
         <v>55</v>
       </c>
-      <c r="U19" s="50">
+      <c r="U19" s="27">
         <v>90</v>
       </c>
     </row>
-    <row r="20" spans="1:29" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="26"/>
+    <row r="20" spans="1:29" ht="15" customHeight="1">
+      <c r="A20" s="30"/>
       <c r="B20" s="6">
         <v>6</v>
       </c>
@@ -3654,21 +3376,21 @@
         <f>(-0.35*C20)+E20</f>
         <v>-26.854563932884545</v>
       </c>
-      <c r="T20" s="33" t="s">
+      <c r="T20" s="37" t="s">
         <v>36</v>
       </c>
-      <c r="U20" s="34"/>
-      <c r="W20" s="26" t="s">
+      <c r="U20" s="38"/>
+      <c r="W20" s="30" t="s">
         <v>0</v>
       </c>
-      <c r="X20" s="26"/>
-      <c r="Z20" s="26" t="s">
+      <c r="X20" s="30"/>
+      <c r="Z20" s="30" t="s">
         <v>1</v>
       </c>
-      <c r="AA20" s="26"/>
-      <c r="AB20" s="26"/>
-    </row>
-    <row r="21" spans="1:29" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="AA20" s="30"/>
+      <c r="AB20" s="30"/>
+    </row>
+    <row r="21" spans="1:29" ht="15" customHeight="1">
       <c r="A21" s="20"/>
       <c r="B21" s="20"/>
       <c r="C21" s="21"/>
@@ -3682,11 +3404,11 @@
       <c r="U21" s="5">
         <v>0</v>
       </c>
-      <c r="W21" s="39">
+      <c r="W21" s="43">
         <f>U25+U3</f>
         <v>0</v>
       </c>
-      <c r="X21" s="40"/>
+      <c r="X21" s="44"/>
       <c r="Z21" s="15">
         <f>COS(Y5)*COS(Y4)</f>
         <v>1</v>
@@ -3700,8 +3422,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:29" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="27" t="s">
+    <row r="22" spans="1:29" ht="15" customHeight="1">
+      <c r="A22" s="31" t="s">
         <v>11</v>
       </c>
       <c r="B22" s="6">
@@ -3733,11 +3455,11 @@
       <c r="U22" s="5">
         <v>0</v>
       </c>
-      <c r="W22" s="41">
+      <c r="W22" s="45">
         <f>U26+U4</f>
         <v>0</v>
       </c>
-      <c r="X22" s="42"/>
+      <c r="X22" s="46"/>
       <c r="Z22" s="5">
         <f>SIN(Y5)*COS(Y4)</f>
         <v>0</v>
@@ -3751,8 +3473,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:29" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="28"/>
+    <row r="23" spans="1:29" ht="15" customHeight="1">
+      <c r="A23" s="32"/>
       <c r="B23" s="6">
         <v>2</v>
       </c>
@@ -3782,11 +3504,11 @@
       <c r="U23" s="5">
         <v>0</v>
       </c>
-      <c r="W23" s="39">
+      <c r="W23" s="43">
         <f>U27+U5</f>
         <v>144</v>
       </c>
-      <c r="X23" s="39"/>
+      <c r="X23" s="43"/>
       <c r="Z23" s="5">
         <f>-SIN(Y4)</f>
         <v>0</v>
@@ -3800,8 +3522,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:29" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="28"/>
+    <row r="24" spans="1:29" ht="15" customHeight="1">
+      <c r="A24" s="32"/>
       <c r="B24" s="6">
         <v>3</v>
       </c>
@@ -3825,10 +3547,10 @@
         <f t="shared" si="8"/>
         <v>193.10304076329146</v>
       </c>
-      <c r="T24" s="33" t="s">
+      <c r="T24" s="37" t="s">
         <v>37</v>
       </c>
-      <c r="U24" s="34"/>
+      <c r="U24" s="38"/>
       <c r="W24" s="19"/>
       <c r="X24" s="23"/>
       <c r="Y24" s="17"/>
@@ -3836,8 +3558,8 @@
       <c r="AA24" s="14"/>
       <c r="AB24" s="14"/>
     </row>
-    <row r="25" spans="1:29" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="28"/>
+    <row r="25" spans="1:29" ht="15" customHeight="1">
+      <c r="A25" s="32"/>
       <c r="B25" s="6">
         <v>4</v>
       </c>
@@ -3868,8 +3590,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:29" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="28"/>
+    <row r="26" spans="1:29" ht="15" customHeight="1">
+      <c r="A26" s="32"/>
       <c r="B26" s="6">
         <v>5</v>
       </c>
@@ -3900,8 +3622,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:29" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="28"/>
+    <row r="27" spans="1:29" ht="15" customHeight="1">
+      <c r="A27" s="32"/>
       <c r="B27" s="6">
         <v>6</v>
       </c>
@@ -3939,8 +3661,8 @@
       <c r="AB27" s="24"/>
       <c r="AC27" s="24"/>
     </row>
-    <row r="28" spans="1:29" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="29"/>
+    <row r="28" spans="1:29" ht="15" customHeight="1">
+      <c r="A28" s="33"/>
       <c r="B28" s="6" t="s">
         <v>39</v>
       </c>
@@ -3955,8 +3677,26 @@
         <f>(-0.35*C22)+E22</f>
         <v>121.75152316959309</v>
       </c>
-    </row>
-    <row r="29" spans="1:29" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="X28" s="24" t="s">
+        <v>42</v>
+      </c>
+      <c r="Y28" s="24" t="s">
+        <v>43</v>
+      </c>
+      <c r="Z28" s="24" t="s">
+        <v>44</v>
+      </c>
+      <c r="AA28" s="24" t="s">
+        <v>45</v>
+      </c>
+      <c r="AB28" s="24" t="s">
+        <v>46</v>
+      </c>
+      <c r="AC28" s="24" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="29" spans="1:29" ht="15" customHeight="1">
       <c r="A29" s="20"/>
       <c r="B29" s="20"/>
       <c r="C29" s="21"/>
@@ -3966,37 +3706,55 @@
       <c r="G29" s="22"/>
       <c r="I29" s="17"/>
       <c r="J29" s="17"/>
-    </row>
-    <row r="30" spans="1:29" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="27" t="s">
+      <c r="X29">
+        <v>50</v>
+      </c>
+      <c r="Y29">
+        <v>50</v>
+      </c>
+      <c r="Z29">
+        <v>50</v>
+      </c>
+      <c r="AA29">
+        <v>45</v>
+      </c>
+      <c r="AB29">
+        <v>45</v>
+      </c>
+      <c r="AC29">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="30" spans="1:29" ht="15" customHeight="1">
+      <c r="A30" s="31" t="s">
         <v>52</v>
       </c>
       <c r="B30" s="6">
         <v>1</v>
       </c>
-      <c r="C30" s="46">
+      <c r="C30" s="50">
         <f>SQRT(POWER($C22-$C2,2)+POWER($D22-$D2,2)+POWER($E22-$E2,2))</f>
         <v>165.06110118251149</v>
       </c>
-      <c r="D30" s="47"/>
-      <c r="E30" s="47"/>
-      <c r="F30" s="47"/>
-      <c r="G30" s="48"/>
-    </row>
-    <row r="31" spans="1:29" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="28"/>
+      <c r="D30" s="51"/>
+      <c r="E30" s="51"/>
+      <c r="F30" s="51"/>
+      <c r="G30" s="52"/>
+    </row>
+    <row r="31" spans="1:29" ht="15" customHeight="1">
+      <c r="A31" s="32"/>
       <c r="B31" s="6">
         <v>2</v>
       </c>
-      <c r="C31" s="46">
+      <c r="C31" s="50">
         <f>SQRT(POWER($C23-$C3,2)+POWER($D23-$D3,2)+POWER($E23-$E3,2))</f>
         <v>165.06110118251149</v>
       </c>
-      <c r="D31" s="47"/>
-      <c r="E31" s="47"/>
-      <c r="F31" s="47"/>
-      <c r="G31" s="48"/>
-      <c r="T31" s="26" t="s">
+      <c r="D31" s="51"/>
+      <c r="E31" s="51"/>
+      <c r="F31" s="51"/>
+      <c r="G31" s="52"/>
+      <c r="T31" s="30" t="s">
         <v>34</v>
       </c>
       <c r="U31" s="6">
@@ -4007,20 +3765,20 @@
         <v>-4278.8328764167018</v>
       </c>
     </row>
-    <row r="32" spans="1:29" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="28"/>
+    <row r="32" spans="1:29" ht="15" customHeight="1">
+      <c r="A32" s="32"/>
       <c r="B32" s="6">
         <v>3</v>
       </c>
-      <c r="C32" s="46">
+      <c r="C32" s="50">
         <f t="shared" ref="C32:C34" si="9">SQRT(POWER($C24-$C4,2)+POWER($D24-$D4,2)+POWER($E24-$E4,2))</f>
         <v>165.06110118251144</v>
       </c>
-      <c r="D32" s="47"/>
-      <c r="E32" s="47"/>
-      <c r="F32" s="47"/>
-      <c r="G32" s="48"/>
-      <c r="T32" s="26"/>
+      <c r="D32" s="51"/>
+      <c r="E32" s="51"/>
+      <c r="F32" s="51"/>
+      <c r="G32" s="52"/>
+      <c r="T32" s="30"/>
       <c r="U32" s="6">
         <v>2</v>
       </c>
@@ -4029,20 +3787,20 @@
         <v>-4278.8328764167054</v>
       </c>
     </row>
-    <row r="33" spans="1:29" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="28"/>
+    <row r="33" spans="1:22" ht="15" customHeight="1">
+      <c r="A33" s="32"/>
       <c r="B33" s="6">
         <v>4</v>
       </c>
-      <c r="C33" s="46">
+      <c r="C33" s="50">
         <f t="shared" si="9"/>
         <v>165.06110118251149</v>
       </c>
-      <c r="D33" s="47"/>
-      <c r="E33" s="47"/>
-      <c r="F33" s="47"/>
-      <c r="G33" s="48"/>
-      <c r="T33" s="26"/>
+      <c r="D33" s="51"/>
+      <c r="E33" s="51"/>
+      <c r="F33" s="51"/>
+      <c r="G33" s="52"/>
+      <c r="T33" s="30"/>
       <c r="U33" s="6">
         <v>3</v>
       </c>
@@ -4051,20 +3809,20 @@
         <v>-4278.83287641672</v>
       </c>
     </row>
-    <row r="34" spans="1:29" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="28"/>
+    <row r="34" spans="1:22" ht="15" customHeight="1">
+      <c r="A34" s="32"/>
       <c r="B34" s="6">
         <v>5</v>
       </c>
-      <c r="C34" s="46">
+      <c r="C34" s="50">
         <f t="shared" si="9"/>
         <v>165.06110118251146</v>
       </c>
-      <c r="D34" s="47"/>
-      <c r="E34" s="47"/>
-      <c r="F34" s="47"/>
-      <c r="G34" s="48"/>
-      <c r="T34" s="26"/>
+      <c r="D34" s="51"/>
+      <c r="E34" s="51"/>
+      <c r="F34" s="51"/>
+      <c r="G34" s="52"/>
+      <c r="T34" s="30"/>
       <c r="U34" s="6">
         <v>4</v>
       </c>
@@ -4073,20 +3831,20 @@
         <v>-4278.8328764167018</v>
       </c>
     </row>
-    <row r="35" spans="1:29" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="29"/>
+    <row r="35" spans="1:22" ht="15" customHeight="1">
+      <c r="A35" s="33"/>
       <c r="B35" s="6">
         <v>6</v>
       </c>
-      <c r="C35" s="46">
+      <c r="C35" s="50">
         <f>SQRT(POWER($C27-$C7,2)+POWER($D27-$D7,2)+POWER($E27-$E7,2))</f>
         <v>165.06110118251146</v>
       </c>
-      <c r="D35" s="47"/>
-      <c r="E35" s="47"/>
-      <c r="F35" s="47"/>
-      <c r="G35" s="48"/>
-      <c r="T35" s="26"/>
+      <c r="D35" s="51"/>
+      <c r="E35" s="51"/>
+      <c r="F35" s="51"/>
+      <c r="G35" s="52"/>
+      <c r="T35" s="30"/>
       <c r="U35" s="6">
         <v>5</v>
       </c>
@@ -4095,7 +3853,7 @@
         <v>-4278.8328764167127</v>
       </c>
     </row>
-    <row r="36" spans="1:29" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:22" ht="15" customHeight="1">
       <c r="A36" s="21"/>
       <c r="B36" s="21"/>
       <c r="C36" s="21"/>
@@ -4103,7 +3861,7 @@
       <c r="E36" s="21"/>
       <c r="F36" s="21"/>
       <c r="G36" s="21"/>
-      <c r="T36" s="26"/>
+      <c r="T36" s="30"/>
       <c r="U36" s="6">
         <v>6</v>
       </c>
@@ -4112,8 +3870,8 @@
         <v>-4278.832876416709</v>
       </c>
     </row>
-    <row r="37" spans="1:29" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A37" s="27" t="s">
+    <row r="37" spans="1:22" ht="15" customHeight="1">
+      <c r="A37" s="31" t="s">
         <v>53</v>
       </c>
       <c r="B37" s="6">
@@ -4139,7 +3897,7 @@
         <f>G22</f>
         <v>121.75152316959309</v>
       </c>
-      <c r="T37" s="26" t="s">
+      <c r="T37" s="30" t="s">
         <v>40</v>
       </c>
       <c r="U37" s="6">
@@ -4150,8 +3908,8 @@
         <v>11520</v>
       </c>
     </row>
-    <row r="38" spans="1:29" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A38" s="28"/>
+    <row r="38" spans="1:22" ht="15" customHeight="1">
+      <c r="A38" s="32"/>
       <c r="B38" s="6"/>
       <c r="C38" s="11">
         <f>C2</f>
@@ -4173,7 +3931,7 @@
         <f>G2</f>
         <v>5.9475624695284148</v>
       </c>
-      <c r="T38" s="26"/>
+      <c r="T38" s="30"/>
       <c r="U38" s="6">
         <v>2</v>
       </c>
@@ -4182,15 +3940,15 @@
         <v>11520</v>
       </c>
     </row>
-    <row r="39" spans="1:29" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A39" s="28"/>
+    <row r="39" spans="1:22" ht="15" customHeight="1">
+      <c r="A39" s="32"/>
       <c r="B39" s="6"/>
       <c r="C39" s="11"/>
       <c r="D39" s="11"/>
       <c r="E39" s="11"/>
       <c r="F39" s="11"/>
       <c r="G39" s="11"/>
-      <c r="T39" s="26"/>
+      <c r="T39" s="30"/>
       <c r="U39" s="6">
         <v>3</v>
       </c>
@@ -4199,8 +3957,8 @@
         <v>11520</v>
       </c>
     </row>
-    <row r="40" spans="1:29" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A40" s="28"/>
+    <row r="40" spans="1:22" ht="15" customHeight="1">
+      <c r="A40" s="32"/>
       <c r="B40" s="6">
         <v>2</v>
       </c>
@@ -4224,7 +3982,7 @@
         <f>G23</f>
         <v>193.10304076329146</v>
       </c>
-      <c r="T40" s="26"/>
+      <c r="T40" s="30"/>
       <c r="U40" s="6">
         <v>4</v>
       </c>
@@ -4233,8 +3991,8 @@
         <v>11520</v>
       </c>
     </row>
-    <row r="41" spans="1:29" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A41" s="28"/>
+    <row r="41" spans="1:22" ht="15" customHeight="1">
+      <c r="A41" s="32"/>
       <c r="B41" s="6"/>
       <c r="C41" s="11">
         <f>C3</f>
@@ -4256,7 +4014,7 @@
         <f>G3</f>
         <v>33.675639555383249</v>
       </c>
-      <c r="T41" s="26"/>
+      <c r="T41" s="30"/>
       <c r="U41" s="6">
         <v>5</v>
       </c>
@@ -4265,15 +4023,15 @@
         <v>11520</v>
       </c>
     </row>
-    <row r="42" spans="1:29" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A42" s="28"/>
+    <row r="42" spans="1:22" ht="15" customHeight="1">
+      <c r="A42" s="32"/>
       <c r="B42" s="6"/>
       <c r="C42" s="11"/>
       <c r="D42" s="11"/>
       <c r="E42" s="11"/>
       <c r="F42" s="11"/>
       <c r="G42" s="11"/>
-      <c r="T42" s="26"/>
+      <c r="T42" s="30"/>
       <c r="U42" s="6">
         <v>6</v>
       </c>
@@ -4282,8 +4040,8 @@
         <v>11520</v>
       </c>
     </row>
-    <row r="43" spans="1:29" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A43" s="28"/>
+    <row r="43" spans="1:22" ht="15" customHeight="1">
+      <c r="A43" s="32"/>
       <c r="B43" s="6">
         <v>3</v>
       </c>
@@ -4307,7 +4065,7 @@
         <f>G24</f>
         <v>193.10304076329146</v>
       </c>
-      <c r="T43" s="26" t="s">
+      <c r="T43" s="30" t="s">
         <v>41</v>
       </c>
       <c r="U43" s="6">
@@ -4318,8 +4076,8 @@
         <v>-5405.9354330321594</v>
       </c>
     </row>
-    <row r="44" spans="1:29" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A44" s="28"/>
+    <row r="44" spans="1:22" ht="15" customHeight="1">
+      <c r="A44" s="32"/>
       <c r="B44" s="6"/>
       <c r="C44" s="11">
         <f>C4</f>
@@ -4341,7 +4099,7 @@
         <f>G4</f>
         <v>33.67563955538327</v>
       </c>
-      <c r="T44" s="26"/>
+      <c r="T44" s="30"/>
       <c r="U44" s="6">
         <v>2</v>
       </c>
@@ -4350,15 +4108,15 @@
         <v>-5405.9354330321567</v>
       </c>
     </row>
-    <row r="45" spans="1:29" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A45" s="28"/>
+    <row r="45" spans="1:22" ht="15" customHeight="1">
+      <c r="A45" s="32"/>
       <c r="B45" s="6"/>
       <c r="C45" s="11"/>
       <c r="D45" s="11"/>
       <c r="E45" s="11"/>
       <c r="F45" s="11"/>
       <c r="G45" s="11"/>
-      <c r="T45" s="26"/>
+      <c r="T45" s="30"/>
       <c r="U45" s="6">
         <v>3</v>
       </c>
@@ -4367,8 +4125,8 @@
         <v>-5405.9354330321503</v>
       </c>
     </row>
-    <row r="46" spans="1:29" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A46" s="28"/>
+    <row r="46" spans="1:22" ht="15" customHeight="1">
+      <c r="A46" s="32"/>
       <c r="B46" s="6">
         <v>4</v>
       </c>
@@ -4392,7 +4150,7 @@
         <f>G25</f>
         <v>121.75152316959307</v>
       </c>
-      <c r="T46" s="26"/>
+      <c r="T46" s="30"/>
       <c r="U46" s="6">
         <v>4</v>
       </c>
@@ -4401,8 +4159,8 @@
         <v>-5405.9354330321594</v>
       </c>
     </row>
-    <row r="47" spans="1:29" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A47" s="28"/>
+    <row r="47" spans="1:22" ht="15" customHeight="1">
+      <c r="A47" s="32"/>
       <c r="B47" s="6"/>
       <c r="C47" s="11">
         <f>C5</f>
@@ -4424,7 +4182,7 @@
         <f>G5</f>
         <v>5.9475624695283997</v>
       </c>
-      <c r="T47" s="26"/>
+      <c r="T47" s="30"/>
       <c r="U47" s="6">
         <v>5</v>
       </c>
@@ -4433,15 +4191,15 @@
         <v>-5405.935433032153</v>
       </c>
     </row>
-    <row r="48" spans="1:29" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A48" s="28"/>
+    <row r="48" spans="1:22" ht="15" customHeight="1">
+      <c r="A48" s="32"/>
       <c r="B48" s="6"/>
       <c r="C48" s="11"/>
       <c r="D48" s="11"/>
       <c r="E48" s="11"/>
       <c r="F48" s="11"/>
       <c r="G48" s="11"/>
-      <c r="T48" s="26"/>
+      <c r="T48" s="30"/>
       <c r="U48" s="6">
         <v>6</v>
       </c>
@@ -4449,27 +4207,9 @@
         <f>2*$U$14*((COS(AC$17)*(C27-C7))+(SIN(AC$17)*(D27-D7)))</f>
         <v>-5405.9354330321557</v>
       </c>
-      <c r="X48" s="24" t="s">
-        <v>42</v>
-      </c>
-      <c r="Y48" s="24" t="s">
-        <v>43</v>
-      </c>
-      <c r="Z48" s="24" t="s">
-        <v>44</v>
-      </c>
-      <c r="AA48" s="24" t="s">
-        <v>45</v>
-      </c>
-      <c r="AB48" s="24" t="s">
-        <v>46</v>
-      </c>
-      <c r="AC48" s="24" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="49" spans="1:29" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A49" s="28"/>
+    </row>
+    <row r="49" spans="1:23" ht="15" customHeight="1">
+      <c r="A49" s="32"/>
       <c r="B49" s="6">
         <v>5</v>
       </c>
@@ -4493,27 +4233,9 @@
         <f>G26</f>
         <v>117.14543606711544</v>
       </c>
-      <c r="X49">
-        <v>50</v>
-      </c>
-      <c r="Y49">
-        <v>50</v>
-      </c>
-      <c r="Z49">
-        <v>50</v>
-      </c>
-      <c r="AA49">
-        <v>45</v>
-      </c>
-      <c r="AB49">
-        <v>45</v>
-      </c>
-      <c r="AC49">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="50" spans="1:29" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A50" s="28"/>
+    </row>
+    <row r="50" spans="1:23" ht="15" customHeight="1">
+      <c r="A50" s="32"/>
       <c r="B50" s="6"/>
       <c r="C50" s="11">
         <f>C6</f>
@@ -4536,8 +4258,8 @@
         <v>-39.623202024911656</v>
       </c>
     </row>
-    <row r="51" spans="1:29" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A51" s="28"/>
+    <row r="51" spans="1:23" ht="15" customHeight="1">
+      <c r="A51" s="32"/>
       <c r="B51" s="6"/>
       <c r="C51" s="11"/>
       <c r="D51" s="11"/>
@@ -4545,8 +4267,8 @@
       <c r="F51" s="11"/>
       <c r="G51" s="11"/>
     </row>
-    <row r="52" spans="1:29" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A52" s="28"/>
+    <row r="52" spans="1:23" ht="15" customHeight="1">
+      <c r="A52" s="32"/>
       <c r="B52" s="6">
         <v>6</v>
       </c>
@@ -4571,8 +4293,8 @@
         <v>117.14543606711545</v>
       </c>
     </row>
-    <row r="53" spans="1:29" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A53" s="29"/>
+    <row r="53" spans="1:23" ht="15" customHeight="1">
+      <c r="A53" s="33"/>
       <c r="B53" s="6"/>
       <c r="C53" s="11">
         <f>C7</f>
@@ -4595,7 +4317,7 @@
         <v>-39.623202024911656</v>
       </c>
     </row>
-    <row r="54" spans="1:29" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:23" ht="15" customHeight="1">
       <c r="A54" s="20"/>
       <c r="B54" s="20"/>
       <c r="C54" s="21"/>
@@ -4604,129 +4326,133 @@
       <c r="F54" s="22"/>
       <c r="G54" s="22"/>
     </row>
-    <row r="55" spans="1:29" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A55" s="27" t="s">
+    <row r="55" spans="1:23" ht="15" customHeight="1">
+      <c r="A55" s="31" t="s">
         <v>38</v>
       </c>
       <c r="B55" s="6">
         <v>1</v>
       </c>
-      <c r="C55" s="41">
-        <f t="shared" ref="C55:C60" si="11">ASIN(V31/(SQRT(POWER(V37,2)+POWER(V43,2))))-ATAN(V43/V37)</f>
+      <c r="C55" s="45">
+        <f>ASIN(V31/(SQRT(POWER(V37,2)+POWER(V43,2))))-ATAN(V43/V37)</f>
         <v>9.5832207228700061E-2</v>
       </c>
-      <c r="D55" s="37"/>
-      <c r="E55" s="37">
-        <f t="shared" ref="E55:E60" si="12">DEGREES(C55)</f>
+      <c r="D55" s="41"/>
+      <c r="E55" s="41">
+        <f t="shared" ref="E55:E60" si="11">DEGREES(C55)</f>
         <v>5.4907810156276122</v>
       </c>
-      <c r="F55" s="37"/>
-      <c r="G55" s="51">
-        <f>((E55-$U$18)*($U$11-$U$10))/($U$19-$U$18)+$U$10</f>
-        <v>388.72695253906903</v>
-      </c>
-    </row>
-    <row r="56" spans="1:29" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A56" s="28"/>
+      <c r="F55" s="41"/>
+      <c r="G55" s="28" t="e" cm="1">
+        <f t="array" aca="1" ref="G55" ca="1">MAPVALUE(E55, $U$18,$U$19,$U$10,$U$11)</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="H55" t="e" cm="1">
+        <f t="array" aca="1" ref="H55" ca="1">MAPVALUE(E55, $U$18,$U$19,$U$10,$U$11)</f>
+        <v>#NAME?</v>
+      </c>
+    </row>
+    <row r="56" spans="1:23" ht="15" customHeight="1">
+      <c r="A56" s="32"/>
       <c r="B56" s="6">
         <v>2</v>
       </c>
-      <c r="C56" s="41">
+      <c r="C56" s="45">
+        <f t="shared" ref="C55:C60" si="12">ASIN(V32/(SQRT(POWER(V38,2)+POWER(V44,2))))-ATAN(V44/V38)</f>
+        <v>9.5832207228699617E-2</v>
+      </c>
+      <c r="D56" s="41"/>
+      <c r="E56" s="41">
         <f t="shared" si="11"/>
-        <v>9.5832207228699617E-2</v>
-      </c>
-      <c r="D56" s="37"/>
-      <c r="E56" s="37">
-        <f t="shared" si="12"/>
         <v>5.4907810156275874</v>
       </c>
-      <c r="F56" s="37"/>
-      <c r="G56" s="51">
-        <f t="shared" ref="G56:G60" si="13">((E56-$U$18)*($U$11-$U$10))/($U$19-$U$18)+$U$10</f>
-        <v>388.72695253906898</v>
-      </c>
-    </row>
-    <row r="57" spans="1:29" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A57" s="28"/>
+      <c r="F56" s="41"/>
+      <c r="G56" s="28" t="e" cm="1">
+        <f t="array" aca="1" ref="G56" ca="1">MAPVALUE(E56, $U$18,$U$19,$U$11,$U$10)</f>
+        <v>#NAME?</v>
+      </c>
+    </row>
+    <row r="57" spans="1:23" ht="15" customHeight="1">
+      <c r="A57" s="32"/>
       <c r="B57" s="6">
         <v>3</v>
       </c>
-      <c r="C57" s="41">
+      <c r="C57" s="45">
+        <f>ASIN(V33/(SQRT(POWER(V39,2)+POWER(V45,2))))-ATAN(V45/V39)</f>
+        <v>9.5832207228697841E-2</v>
+      </c>
+      <c r="D57" s="41"/>
+      <c r="E57" s="41">
         <f t="shared" si="11"/>
-        <v>9.5832207228697841E-2</v>
-      </c>
-      <c r="D57" s="37"/>
-      <c r="E57" s="37">
-        <f t="shared" si="12"/>
         <v>5.4907810156274852</v>
       </c>
-      <c r="F57" s="37"/>
-      <c r="G57" s="51">
-        <f t="shared" si="13"/>
-        <v>388.72695253906875</v>
-      </c>
-    </row>
-    <row r="58" spans="1:29" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A58" s="28"/>
+      <c r="F57" s="41"/>
+      <c r="G57" s="28" t="e" cm="1">
+        <f t="array" aca="1" ref="G57" ca="1">MAPVALUE(E57, $U$18,$U$19,$U$10,$U$11)</f>
+        <v>#NAME?</v>
+      </c>
+    </row>
+    <row r="58" spans="1:23" ht="15" customHeight="1">
+      <c r="A58" s="32"/>
       <c r="B58" s="6">
         <v>4</v>
       </c>
-      <c r="C58" s="41">
+      <c r="C58" s="45">
+        <f t="shared" si="12"/>
+        <v>9.5832207228700061E-2</v>
+      </c>
+      <c r="D58" s="41"/>
+      <c r="E58" s="41">
         <f t="shared" si="11"/>
-        <v>9.5832207228700061E-2</v>
-      </c>
-      <c r="D58" s="37"/>
-      <c r="E58" s="37">
-        <f t="shared" si="12"/>
         <v>5.4907810156276122</v>
       </c>
-      <c r="F58" s="37"/>
-      <c r="G58" s="51">
-        <f t="shared" si="13"/>
-        <v>388.72695253906903</v>
-      </c>
-    </row>
-    <row r="59" spans="1:29" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A59" s="28"/>
+      <c r="F58" s="41"/>
+      <c r="G58" s="28" t="e" cm="1">
+        <f t="array" aca="1" ref="G58" ca="1">MAPVALUE(E58, $U$18,$U$19,$U$11,$U$10)</f>
+        <v>#NAME?</v>
+      </c>
+    </row>
+    <row r="59" spans="1:23" ht="15" customHeight="1">
+      <c r="A59" s="32"/>
       <c r="B59" s="6">
         <v>5</v>
       </c>
-      <c r="C59" s="41">
+      <c r="C59" s="45">
+        <f t="shared" si="12"/>
+        <v>9.5832207228698674E-2</v>
+      </c>
+      <c r="D59" s="41"/>
+      <c r="E59" s="41">
         <f t="shared" si="11"/>
-        <v>9.5832207228698674E-2</v>
-      </c>
-      <c r="D59" s="37"/>
-      <c r="E59" s="37">
-        <f t="shared" si="12"/>
         <v>5.4907810156275332</v>
       </c>
-      <c r="F59" s="37"/>
-      <c r="G59" s="51">
-        <f t="shared" si="13"/>
-        <v>388.72695253906886</v>
-      </c>
-    </row>
-    <row r="60" spans="1:29" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A60" s="29"/>
+      <c r="F59" s="41"/>
+      <c r="G59" s="28" t="e" cm="1">
+        <f t="array" aca="1" ref="G59" ca="1">MAPVALUE(E59, $U$18,$U$19,$U$10,$U$11)</f>
+        <v>#NAME?</v>
+      </c>
+    </row>
+    <row r="60" spans="1:23" ht="15" customHeight="1">
+      <c r="A60" s="33"/>
       <c r="B60" s="6">
         <v>6</v>
       </c>
-      <c r="C60" s="41">
+      <c r="C60" s="45">
+        <f t="shared" si="12"/>
+        <v>9.5832207228699173E-2</v>
+      </c>
+      <c r="D60" s="41"/>
+      <c r="E60" s="41">
         <f t="shared" si="11"/>
-        <v>9.5832207228699173E-2</v>
-      </c>
-      <c r="D60" s="37"/>
-      <c r="E60" s="37">
-        <f t="shared" si="12"/>
         <v>5.4907810156275616</v>
       </c>
-      <c r="F60" s="37"/>
-      <c r="G60" s="51">
-        <f t="shared" si="13"/>
-        <v>388.72695253906892</v>
-      </c>
-    </row>
-    <row r="61" spans="1:29" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="F60" s="41"/>
+      <c r="G60" s="28" t="e" cm="1">
+        <f t="array" aca="1" ref="G60" ca="1">MAPVALUE(E60, $U$18,$U$19,$U$11,$U$10)</f>
+        <v>#NAME?</v>
+      </c>
+    </row>
+    <row r="61" spans="1:23" ht="15" customHeight="1">
       <c r="A61" s="20"/>
       <c r="B61" s="20"/>
       <c r="C61" s="21"/>
@@ -4750,9 +4476,25 @@
       <c r="O61" s="25" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="62" spans="1:29" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A62" s="43" t="s">
+      <c r="R61" s="1"/>
+      <c r="S61" s="29" t="s">
+        <v>2</v>
+      </c>
+      <c r="T61" s="29" t="s">
+        <v>3</v>
+      </c>
+      <c r="U61" s="29" t="s">
+        <v>4</v>
+      </c>
+      <c r="V61" s="29" t="s">
+        <v>8</v>
+      </c>
+      <c r="W61" s="29" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="62" spans="1:23" ht="15" customHeight="1">
+      <c r="A62" s="47" t="s">
         <v>50</v>
       </c>
       <c r="B62" s="6">
@@ -4771,14 +4513,14 @@
         <v>3.8274236163370832</v>
       </c>
       <c r="F62" s="11">
-        <f t="shared" ref="F62:F77" si="14">(-0.35*C62)+D62</f>
+        <f t="shared" ref="F62:F77" si="13">(-0.35*C62)+D62</f>
         <v>158.83625015431414</v>
       </c>
       <c r="G62" s="11">
-        <f t="shared" ref="G62:G77" si="15">(-0.35*C62)+E62</f>
+        <f t="shared" ref="G62:G77" si="14">(-0.35*C62)+E62</f>
         <v>21.843710432906658</v>
       </c>
-      <c r="I62" s="27" t="s">
+      <c r="I62" s="31" t="s">
         <v>51</v>
       </c>
       <c r="J62" s="25">
@@ -4789,24 +4531,50 @@
         <v>-51.475105190198789</v>
       </c>
       <c r="L62" s="11">
-        <f t="shared" ref="L62:O62" si="16">D62</f>
+        <f t="shared" ref="L62:O62" si="15">D62</f>
         <v>140.81996333774458</v>
       </c>
       <c r="M62" s="11">
-        <f t="shared" si="16"/>
+        <f t="shared" si="15"/>
         <v>3.8274236163370832</v>
       </c>
       <c r="N62" s="11">
-        <f t="shared" si="16"/>
+        <f t="shared" si="15"/>
         <v>158.83625015431414</v>
       </c>
       <c r="O62" s="11">
-        <f t="shared" si="16"/>
+        <f t="shared" si="15"/>
         <v>21.843710432906658</v>
       </c>
-    </row>
-    <row r="63" spans="1:29" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A63" s="44"/>
+      <c r="Q62" s="31" t="s">
+        <v>34</v>
+      </c>
+      <c r="R62" s="29">
+        <v>1</v>
+      </c>
+      <c r="S62" s="11">
+        <f>C22-C2</f>
+        <v>80.560112285529513</v>
+      </c>
+      <c r="T62" s="11">
+        <f>D22-D2</f>
+        <v>4.385821716186868</v>
+      </c>
+      <c r="U62" s="11">
+        <f>E22-E2</f>
+        <v>144</v>
+      </c>
+      <c r="V62" s="11">
+        <f>(-0.35*S62)+T62</f>
+        <v>-23.810217583748461</v>
+      </c>
+      <c r="W62" s="11">
+        <f>(-0.35*S62)+U62</f>
+        <v>115.80396070006466</v>
+      </c>
+    </row>
+    <row r="63" spans="1:23" ht="15" customHeight="1">
+      <c r="A63" s="48"/>
       <c r="B63" s="6"/>
       <c r="C63" s="11">
         <f>C2</f>
@@ -4828,47 +4596,95 @@
         <f>G2</f>
         <v>5.9475624695284148</v>
       </c>
-      <c r="I63" s="28"/>
+      <c r="I63" s="32"/>
       <c r="J63" s="25"/>
       <c r="K63" s="11">
         <f>C22</f>
         <v>63.567076658305467</v>
       </c>
       <c r="L63" s="11">
-        <f t="shared" ref="L63:O63" si="17">D22</f>
+        <f t="shared" ref="L63:O63" si="16">D22</f>
         <v>125.29755290953258</v>
       </c>
       <c r="M63" s="11">
-        <f t="shared" si="17"/>
+        <f t="shared" si="16"/>
         <v>144</v>
       </c>
       <c r="N63" s="11">
-        <f t="shared" si="17"/>
+        <f t="shared" si="16"/>
         <v>103.04907607912567</v>
       </c>
       <c r="O63" s="11">
-        <f t="shared" si="17"/>
+        <f t="shared" si="16"/>
         <v>121.75152316959309</v>
       </c>
-    </row>
-    <row r="64" spans="1:29" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A64" s="44"/>
+      <c r="Q63" s="32"/>
+      <c r="R63" s="29">
+        <v>2</v>
+      </c>
+      <c r="S63" s="11">
+        <f t="shared" ref="S63:S67" si="17">C23-C3</f>
+        <v>-44.07828916545202</v>
+      </c>
+      <c r="T63" s="11">
+        <f t="shared" ref="T63:T67" si="18">D23-D3</f>
+        <v>-67.574192912901964</v>
+      </c>
+      <c r="U63" s="11">
+        <f t="shared" ref="U63:U67" si="19">E23-E3</f>
+        <v>144</v>
+      </c>
+      <c r="V63" s="11">
+        <f t="shared" ref="V63:V67" si="20">(-0.35*S63)+T63</f>
+        <v>-52.14679170499376</v>
+      </c>
+      <c r="W63" s="11">
+        <f t="shared" ref="W63:W67" si="21">(-0.35*S63)+U63</f>
+        <v>159.42740120790822</v>
+      </c>
+    </row>
+    <row r="64" spans="1:23" ht="15" customHeight="1">
+      <c r="A64" s="48"/>
       <c r="B64" s="6"/>
       <c r="C64" s="1"/>
       <c r="D64" s="1"/>
       <c r="E64" s="1"/>
       <c r="F64" s="11"/>
       <c r="G64" s="11"/>
-      <c r="I64" s="28"/>
+      <c r="I64" s="32"/>
       <c r="J64" s="25"/>
       <c r="K64" s="11"/>
       <c r="L64" s="11"/>
       <c r="M64" s="11"/>
       <c r="N64" s="11"/>
       <c r="O64" s="11"/>
-    </row>
-    <row r="65" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A65" s="44"/>
+      <c r="Q64" s="32"/>
+      <c r="R64" s="29">
+        <v>3</v>
+      </c>
+      <c r="S64" s="11">
+        <f t="shared" si="17"/>
+        <v>-44.078289165451977</v>
+      </c>
+      <c r="T64" s="11">
+        <f t="shared" si="18"/>
+        <v>67.574192912901879</v>
+      </c>
+      <c r="U64" s="11">
+        <f t="shared" si="19"/>
+        <v>144</v>
+      </c>
+      <c r="V64" s="11">
+        <f t="shared" si="20"/>
+        <v>83.001594120810068</v>
+      </c>
+      <c r="W64" s="11">
+        <f t="shared" si="21"/>
+        <v>159.42740120790819</v>
+      </c>
+    </row>
+    <row r="65" spans="1:23" ht="15" customHeight="1">
+      <c r="A65" s="48"/>
       <c r="B65" s="6">
         <v>2</v>
       </c>
@@ -4885,14 +4701,14 @@
         <v>3.8274236163370654</v>
       </c>
       <c r="F65" s="11">
+        <f t="shared" si="13"/>
+        <v>148.66436998144388</v>
+      </c>
+      <c r="G65" s="11">
         <f t="shared" si="14"/>
-        <v>148.66436998144388</v>
-      </c>
-      <c r="G65" s="11">
-        <f t="shared" si="15"/>
         <v>37.503063171720314</v>
       </c>
-      <c r="I65" s="28"/>
+      <c r="I65" s="32"/>
       <c r="J65" s="25">
         <v>2</v>
       </c>
@@ -4901,24 +4717,48 @@
         <v>-96.216113015380728</v>
       </c>
       <c r="L65" s="11">
-        <f t="shared" ref="L65:O65" si="18">D65</f>
+        <f t="shared" ref="L65:O65" si="22">D65</f>
         <v>114.98873042606063</v>
       </c>
       <c r="M65" s="11">
+        <f t="shared" si="22"/>
+        <v>3.8274236163370654</v>
+      </c>
+      <c r="N65" s="11">
+        <f t="shared" si="22"/>
+        <v>148.66436998144388</v>
+      </c>
+      <c r="O65" s="11">
+        <f t="shared" si="22"/>
+        <v>37.503063171720314</v>
+      </c>
+      <c r="Q65" s="32"/>
+      <c r="R65" s="29">
+        <v>4</v>
+      </c>
+      <c r="S65" s="11">
+        <f t="shared" si="17"/>
+        <v>80.560112285529499</v>
+      </c>
+      <c r="T65" s="11">
         <f t="shared" si="18"/>
-        <v>3.8274236163370654</v>
-      </c>
-      <c r="N65" s="11">
-        <f t="shared" si="18"/>
-        <v>148.66436998144388</v>
-      </c>
-      <c r="O65" s="11">
-        <f t="shared" si="18"/>
-        <v>37.503063171720314</v>
-      </c>
-    </row>
-    <row r="66" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A66" s="44"/>
+        <v>-4.3858217161868396</v>
+      </c>
+      <c r="U65" s="11">
+        <f t="shared" si="19"/>
+        <v>144</v>
+      </c>
+      <c r="V65" s="11">
+        <f t="shared" si="20"/>
+        <v>-32.581861016122161</v>
+      </c>
+      <c r="W65" s="11">
+        <f t="shared" si="21"/>
+        <v>115.80396070006468</v>
+      </c>
+    </row>
+    <row r="66" spans="1:23" ht="15" customHeight="1">
+      <c r="A66" s="48"/>
       <c r="B66" s="6"/>
       <c r="C66" s="11">
         <f>C3</f>
@@ -4940,47 +4780,95 @@
         <f>G3</f>
         <v>33.675639555383249</v>
       </c>
-      <c r="I66" s="28"/>
+      <c r="I66" s="32"/>
       <c r="J66" s="25"/>
       <c r="K66" s="11">
         <f>C23</f>
         <v>-140.29440218083275</v>
       </c>
       <c r="L66" s="11">
-        <f t="shared" ref="L66:O66" si="19">D23</f>
+        <f t="shared" ref="L66:O66" si="23">D23</f>
         <v>7.5980732243609284</v>
       </c>
       <c r="M66" s="11">
+        <f t="shared" si="23"/>
+        <v>144</v>
+      </c>
+      <c r="N66" s="11">
+        <f t="shared" si="23"/>
+        <v>56.701113987652391</v>
+      </c>
+      <c r="O66" s="11">
+        <f t="shared" si="23"/>
+        <v>193.10304076329146</v>
+      </c>
+      <c r="Q66" s="32"/>
+      <c r="R66" s="29">
+        <v>5</v>
+      </c>
+      <c r="S66" s="11">
+        <f t="shared" si="17"/>
+        <v>-36.481823120077436</v>
+      </c>
+      <c r="T66" s="11">
+        <f t="shared" si="18"/>
+        <v>-71.960014629088775</v>
+      </c>
+      <c r="U66" s="11">
         <f t="shared" si="19"/>
         <v>144</v>
       </c>
-      <c r="N66" s="11">
-        <f t="shared" si="19"/>
-        <v>56.701113987652391</v>
-      </c>
-      <c r="O66" s="11">
-        <f t="shared" si="19"/>
-        <v>193.10304076329146</v>
-      </c>
-    </row>
-    <row r="67" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A67" s="44"/>
+      <c r="V66" s="11">
+        <f t="shared" si="20"/>
+        <v>-59.191376537061672</v>
+      </c>
+      <c r="W66" s="11">
+        <f t="shared" si="21"/>
+        <v>156.76863809202709</v>
+      </c>
+    </row>
+    <row r="67" spans="1:23" ht="15" customHeight="1">
+      <c r="A67" s="48"/>
       <c r="B67" s="6"/>
       <c r="C67" s="1"/>
       <c r="D67" s="1"/>
       <c r="E67" s="1"/>
       <c r="F67" s="11"/>
       <c r="G67" s="11"/>
-      <c r="I67" s="28"/>
+      <c r="I67" s="32"/>
       <c r="J67" s="25"/>
       <c r="K67" s="11"/>
       <c r="L67" s="11"/>
       <c r="M67" s="11"/>
       <c r="N67" s="11"/>
       <c r="O67" s="11"/>
-    </row>
-    <row r="68" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A68" s="44"/>
+      <c r="Q67" s="32"/>
+      <c r="R67" s="29">
+        <v>6</v>
+      </c>
+      <c r="S67" s="11">
+        <f t="shared" si="17"/>
+        <v>-36.481823120077465</v>
+      </c>
+      <c r="T67" s="11">
+        <f t="shared" si="18"/>
+        <v>71.960014629088789</v>
+      </c>
+      <c r="U67" s="11">
+        <f t="shared" si="19"/>
+        <v>144</v>
+      </c>
+      <c r="V67" s="11">
+        <f t="shared" si="20"/>
+        <v>84.728652721115907</v>
+      </c>
+      <c r="W67" s="11">
+        <f t="shared" si="21"/>
+        <v>156.76863809202712</v>
+      </c>
+    </row>
+    <row r="68" spans="1:23" ht="15" customHeight="1">
+      <c r="A68" s="48"/>
       <c r="B68" s="6">
         <v>3</v>
       </c>
@@ -4997,14 +4885,14 @@
         <v>3.8274236163369943</v>
       </c>
       <c r="F68" s="11">
+        <f t="shared" si="13"/>
+        <v>-81.313090870677314</v>
+      </c>
+      <c r="G68" s="11">
         <f t="shared" si="14"/>
-        <v>-81.313090870677314</v>
-      </c>
-      <c r="G68" s="11">
-        <f t="shared" si="15"/>
         <v>37.503063171720264</v>
       </c>
-      <c r="I68" s="28"/>
+      <c r="I68" s="32"/>
       <c r="J68" s="25">
         <v>3</v>
       </c>
@@ -5013,24 +4901,39 @@
         <v>-96.21611301538077</v>
       </c>
       <c r="L68" s="11">
-        <f t="shared" ref="L68:O68" si="20">D68</f>
+        <f t="shared" ref="L68:O68" si="24">D68</f>
         <v>-114.98873042606058</v>
       </c>
       <c r="M68" s="11">
-        <f t="shared" si="20"/>
+        <f t="shared" si="24"/>
         <v>3.8274236163369943</v>
       </c>
       <c r="N68" s="11">
-        <f t="shared" si="20"/>
+        <f t="shared" si="24"/>
         <v>-81.313090870677314</v>
       </c>
       <c r="O68" s="11">
-        <f t="shared" si="20"/>
+        <f t="shared" si="24"/>
         <v>37.503063171720264</v>
       </c>
-    </row>
-    <row r="69" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A69" s="44"/>
+      <c r="Q68" s="33"/>
+      <c r="R68" s="29" t="s">
+        <v>39</v>
+      </c>
+      <c r="S68" s="1"/>
+      <c r="T68" s="1"/>
+      <c r="U68" s="1"/>
+      <c r="V68" s="11">
+        <f>(-0.35*S62)+T62</f>
+        <v>-23.810217583748461</v>
+      </c>
+      <c r="W68" s="11">
+        <f>(-0.35*S62)+U62</f>
+        <v>115.80396070006466</v>
+      </c>
+    </row>
+    <row r="69" spans="1:23" ht="15" customHeight="1">
+      <c r="A69" s="48"/>
       <c r="B69" s="6"/>
       <c r="C69" s="11">
         <f>C4</f>
@@ -5052,38 +4955,38 @@
         <f>G4</f>
         <v>33.67563955538327</v>
       </c>
-      <c r="I69" s="28"/>
+      <c r="I69" s="32"/>
       <c r="J69" s="25"/>
       <c r="K69" s="11">
         <f>C24</f>
         <v>-140.29440218083275</v>
       </c>
       <c r="L69" s="11">
-        <f t="shared" ref="L69:O69" si="21">D24</f>
+        <f t="shared" ref="L69:O69" si="25">D24</f>
         <v>-7.5980732243609808</v>
       </c>
       <c r="M69" s="11">
-        <f t="shared" si="21"/>
+        <f t="shared" si="25"/>
         <v>144</v>
       </c>
       <c r="N69" s="11">
-        <f t="shared" si="21"/>
+        <f t="shared" si="25"/>
         <v>41.50496753893048</v>
       </c>
       <c r="O69" s="11">
-        <f t="shared" si="21"/>
+        <f t="shared" si="25"/>
         <v>193.10304076329146</v>
       </c>
     </row>
-    <row r="70" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A70" s="44"/>
+    <row r="70" spans="1:23" ht="15" customHeight="1">
+      <c r="A70" s="48"/>
       <c r="B70" s="6"/>
       <c r="C70" s="1"/>
       <c r="D70" s="1"/>
       <c r="E70" s="1"/>
       <c r="F70" s="11"/>
       <c r="G70" s="11"/>
-      <c r="I70" s="28"/>
+      <c r="I70" s="32"/>
       <c r="J70" s="25"/>
       <c r="K70" s="11"/>
       <c r="L70" s="11"/>
@@ -5091,8 +4994,8 @@
       <c r="N70" s="11"/>
       <c r="O70" s="11"/>
     </row>
-    <row r="71" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A71" s="44"/>
+    <row r="71" spans="1:23">
+      <c r="A71" s="48"/>
       <c r="B71" s="6">
         <v>4</v>
       </c>
@@ -5109,14 +5012,14 @@
         <v>3.8274236163370832</v>
       </c>
       <c r="F71" s="11">
+        <f t="shared" si="13"/>
+        <v>-122.80367652117502</v>
+      </c>
+      <c r="G71" s="11">
         <f t="shared" si="14"/>
-        <v>-122.80367652117502</v>
-      </c>
-      <c r="G71" s="11">
-        <f t="shared" si="15"/>
         <v>21.843710432906644</v>
       </c>
-      <c r="I71" s="28"/>
+      <c r="I71" s="32"/>
       <c r="J71" s="25">
         <v>4</v>
       </c>
@@ -5125,15 +5028,15 @@
         <v>-51.475105190198747</v>
       </c>
       <c r="L71" s="11">
-        <f t="shared" ref="L71:N71" si="22">D71</f>
+        <f t="shared" ref="L71:N71" si="26">D71</f>
         <v>-140.81996333774458</v>
       </c>
       <c r="M71" s="11">
-        <f t="shared" si="22"/>
+        <f t="shared" si="26"/>
         <v>3.8274236163370832</v>
       </c>
       <c r="N71" s="11">
-        <f t="shared" si="22"/>
+        <f t="shared" si="26"/>
         <v>-122.80367652117502</v>
       </c>
       <c r="O71" s="11">
@@ -5141,8 +5044,8 @@
         <v>21.843710432906644</v>
       </c>
     </row>
-    <row r="72" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A72" s="44"/>
+    <row r="72" spans="1:23">
+      <c r="A72" s="48"/>
       <c r="B72" s="6"/>
       <c r="C72" s="11">
         <f>C5</f>
@@ -5164,38 +5067,38 @@
         <f>G5</f>
         <v>5.9475624695283997</v>
       </c>
-      <c r="I72" s="28"/>
+      <c r="I72" s="32"/>
       <c r="J72" s="25"/>
       <c r="K72" s="11">
         <f>C25</f>
         <v>63.567076658305503</v>
       </c>
       <c r="L72" s="11">
-        <f t="shared" ref="L72:O72" si="23">D25</f>
+        <f t="shared" ref="L72:O72" si="27">D25</f>
         <v>-125.29755290953256</v>
       </c>
       <c r="M72" s="11">
-        <f t="shared" si="23"/>
+        <f t="shared" si="27"/>
         <v>144</v>
       </c>
       <c r="N72" s="11">
-        <f t="shared" si="23"/>
+        <f t="shared" si="27"/>
         <v>-147.54602973993948</v>
       </c>
       <c r="O72" s="11">
-        <f t="shared" si="23"/>
+        <f t="shared" si="27"/>
         <v>121.75152316959307</v>
       </c>
     </row>
-    <row r="73" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A73" s="44"/>
+    <row r="73" spans="1:23">
+      <c r="A73" s="48"/>
       <c r="B73" s="6"/>
       <c r="C73" s="1"/>
       <c r="D73" s="1"/>
       <c r="E73" s="1"/>
       <c r="F73" s="11"/>
       <c r="G73" s="11"/>
-      <c r="I73" s="28"/>
+      <c r="I73" s="32"/>
       <c r="J73" s="25"/>
       <c r="K73" s="11"/>
       <c r="L73" s="11"/>
@@ -5203,8 +5106,8 @@
       <c r="N73" s="11"/>
       <c r="O73" s="11"/>
     </row>
-    <row r="74" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A74" s="44"/>
+    <row r="74" spans="1:23">
+      <c r="A74" s="48"/>
       <c r="B74" s="6">
         <v>5</v>
       </c>
@@ -5221,14 +5124,14 @@
         <v>3.8274236163370281</v>
       </c>
       <c r="F74" s="11">
+        <f t="shared" si="13"/>
+        <v>-77.523159283636829</v>
+      </c>
+      <c r="G74" s="11">
         <f t="shared" si="14"/>
-        <v>-77.523159283636829</v>
-      </c>
-      <c r="G74" s="11">
-        <f t="shared" si="15"/>
         <v>-47.864502755615796</v>
       </c>
-      <c r="I74" s="28"/>
+      <c r="I74" s="32"/>
       <c r="J74" s="25">
         <v>5</v>
       </c>
@@ -5237,24 +5140,24 @@
         <v>147.6912182055795</v>
       </c>
       <c r="L74" s="11">
-        <f t="shared" ref="L74:O74" si="24">D74</f>
+        <f t="shared" ref="L74:O74" si="28">D74</f>
         <v>-25.831232911683998</v>
       </c>
       <c r="M74" s="11">
-        <f t="shared" si="24"/>
+        <f t="shared" si="28"/>
         <v>3.8274236163370281</v>
       </c>
       <c r="N74" s="11">
-        <f t="shared" si="24"/>
+        <f t="shared" si="28"/>
         <v>-77.523159283636829</v>
       </c>
       <c r="O74" s="11">
-        <f t="shared" si="24"/>
+        <f t="shared" si="28"/>
         <v>-47.864502755615796</v>
       </c>
     </row>
-    <row r="75" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A75" s="44"/>
+    <row r="75" spans="1:23">
+      <c r="A75" s="48"/>
       <c r="B75" s="6"/>
       <c r="C75" s="11">
         <f>C6</f>
@@ -5276,38 +5179,38 @@
         <f>G6</f>
         <v>-39.623202024911656</v>
       </c>
-      <c r="I75" s="28"/>
+      <c r="I75" s="32"/>
       <c r="J75" s="25"/>
       <c r="K75" s="11">
         <f>C26</f>
         <v>76.727325522527309</v>
       </c>
       <c r="L75" s="11">
-        <f t="shared" ref="L75:O75" si="25">D26</f>
+        <f t="shared" ref="L75:O75" si="29">D26</f>
         <v>-117.69947968517164</v>
       </c>
       <c r="M75" s="11">
-        <f t="shared" si="25"/>
+        <f t="shared" si="29"/>
         <v>144</v>
       </c>
       <c r="N75" s="11">
-        <f t="shared" si="25"/>
+        <f t="shared" si="29"/>
         <v>-144.5540436180562</v>
       </c>
       <c r="O75" s="11">
-        <f t="shared" si="25"/>
+        <f t="shared" si="29"/>
         <v>117.14543606711544</v>
       </c>
     </row>
-    <row r="76" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A76" s="44"/>
+    <row r="76" spans="1:23">
+      <c r="A76" s="48"/>
       <c r="B76" s="6"/>
       <c r="C76" s="1"/>
       <c r="D76" s="1"/>
       <c r="E76" s="1"/>
       <c r="F76" s="11"/>
       <c r="G76" s="11"/>
-      <c r="I76" s="28"/>
+      <c r="I76" s="32"/>
       <c r="J76" s="25"/>
       <c r="K76" s="11"/>
       <c r="L76" s="11"/>
@@ -5315,8 +5218,8 @@
       <c r="N76" s="11"/>
       <c r="O76" s="11"/>
     </row>
-    <row r="77" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A77" s="44"/>
+    <row r="77" spans="1:23">
+      <c r="A77" s="48"/>
       <c r="B77" s="6">
         <v>6</v>
       </c>
@@ -5333,14 +5236,14 @@
         <v>3.8274236163370476</v>
       </c>
       <c r="F77" s="11">
+        <f t="shared" si="13"/>
+        <v>-25.860693460268838</v>
+      </c>
+      <c r="G77" s="11">
         <f t="shared" si="14"/>
-        <v>-25.860693460268838</v>
-      </c>
-      <c r="G77" s="11">
-        <f t="shared" si="15"/>
         <v>-47.864502755615774</v>
       </c>
-      <c r="I77" s="28"/>
+      <c r="I77" s="32"/>
       <c r="J77" s="25">
         <v>6</v>
       </c>
@@ -5349,24 +5252,24 @@
         <v>147.6912182055795</v>
       </c>
       <c r="L77" s="11">
-        <f t="shared" ref="L77:O77" si="26">D77</f>
+        <f t="shared" ref="L77:O77" si="30">D77</f>
         <v>25.831232911683987</v>
       </c>
       <c r="M77" s="11">
-        <f t="shared" si="26"/>
+        <f t="shared" si="30"/>
         <v>3.8274236163370476</v>
       </c>
       <c r="N77" s="11">
-        <f t="shared" si="26"/>
+        <f t="shared" si="30"/>
         <v>-25.860693460268838</v>
       </c>
       <c r="O77" s="11">
-        <f t="shared" si="26"/>
+        <f t="shared" si="30"/>
         <v>-47.864502755615774</v>
       </c>
     </row>
-    <row r="78" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A78" s="45"/>
+    <row r="78" spans="1:23">
+      <c r="A78" s="49"/>
       <c r="B78" s="2"/>
       <c r="C78" s="11">
         <f>C7</f>
@@ -5388,110 +5291,110 @@
         <f>G7</f>
         <v>-39.623202024911656</v>
       </c>
-      <c r="I78" s="29"/>
+      <c r="I78" s="33"/>
       <c r="J78" s="25"/>
       <c r="K78" s="11">
         <f>C27</f>
         <v>76.727325522527281</v>
       </c>
       <c r="L78" s="11">
-        <f t="shared" ref="L78:O78" si="27">D27</f>
+        <f t="shared" ref="L78:O78" si="31">D27</f>
         <v>117.69947968517164</v>
       </c>
       <c r="M78" s="11">
-        <f t="shared" si="27"/>
+        <f t="shared" si="31"/>
         <v>144</v>
       </c>
       <c r="N78" s="11">
-        <f t="shared" si="27"/>
+        <f t="shared" si="31"/>
         <v>90.844915752287093</v>
       </c>
       <c r="O78" s="11">
-        <f t="shared" si="27"/>
+        <f t="shared" si="31"/>
         <v>117.14543606711545</v>
       </c>
     </row>
-    <row r="84" spans="6:7" x14ac:dyDescent="0.3">
+    <row r="84" spans="6:7">
       <c r="G84" s="13"/>
     </row>
-    <row r="85" spans="6:7" x14ac:dyDescent="0.3">
+    <row r="85" spans="6:7">
       <c r="G85" s="13"/>
     </row>
-    <row r="86" spans="6:7" x14ac:dyDescent="0.3">
+    <row r="86" spans="6:7">
       <c r="G86" s="13"/>
     </row>
-    <row r="87" spans="6:7" x14ac:dyDescent="0.3">
+    <row r="87" spans="6:7">
       <c r="G87" s="13"/>
     </row>
-    <row r="88" spans="6:7" x14ac:dyDescent="0.3">
+    <row r="88" spans="6:7">
       <c r="G88" s="14"/>
     </row>
-    <row r="89" spans="6:7" x14ac:dyDescent="0.3">
+    <row r="89" spans="6:7">
       <c r="F89" s="14"/>
       <c r="G89" s="14"/>
     </row>
-    <row r="90" spans="6:7" ht="26.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="90" spans="6:7" ht="26.25" customHeight="1">
       <c r="G90" s="14"/>
     </row>
-    <row r="91" spans="6:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="91" spans="6:7" ht="15" customHeight="1">
       <c r="G91" s="14"/>
     </row>
-    <row r="92" spans="6:7" x14ac:dyDescent="0.3">
+    <row r="92" spans="6:7">
       <c r="G92" s="14"/>
     </row>
-    <row r="93" spans="6:7" x14ac:dyDescent="0.3">
+    <row r="93" spans="6:7">
       <c r="G93" s="14"/>
     </row>
-    <row r="107" spans="3:7" x14ac:dyDescent="0.3">
+    <row r="107" spans="3:7">
       <c r="C107" s="18"/>
       <c r="D107" s="18"/>
       <c r="E107" s="18"/>
       <c r="F107" s="18"/>
       <c r="G107" s="18"/>
     </row>
-    <row r="108" spans="3:7" x14ac:dyDescent="0.3">
+    <row r="108" spans="3:7">
       <c r="C108" s="17"/>
       <c r="D108" s="17"/>
       <c r="E108" s="17"/>
       <c r="F108" s="17"/>
       <c r="G108" s="17"/>
     </row>
-    <row r="109" spans="3:7" x14ac:dyDescent="0.3">
+    <row r="109" spans="3:7">
       <c r="C109" s="17"/>
       <c r="D109" s="17"/>
       <c r="E109" s="17"/>
       <c r="F109" s="17"/>
       <c r="G109" s="17"/>
     </row>
-    <row r="110" spans="3:7" x14ac:dyDescent="0.3">
+    <row r="110" spans="3:7">
       <c r="C110" s="18"/>
       <c r="D110" s="18"/>
       <c r="E110" s="18"/>
       <c r="F110" s="18"/>
       <c r="G110" s="18"/>
     </row>
-    <row r="111" spans="3:7" x14ac:dyDescent="0.3">
+    <row r="111" spans="3:7">
       <c r="C111" s="18"/>
       <c r="D111" s="18"/>
       <c r="E111" s="18"/>
       <c r="F111" s="18"/>
       <c r="G111" s="18"/>
     </row>
-    <row r="112" spans="3:7" x14ac:dyDescent="0.3">
+    <row r="112" spans="3:7">
       <c r="C112" s="18"/>
       <c r="D112" s="18"/>
       <c r="E112" s="18"/>
       <c r="F112" s="18"/>
       <c r="G112" s="18"/>
     </row>
-    <row r="113" spans="3:7" x14ac:dyDescent="0.3">
+    <row r="113" spans="3:7">
       <c r="C113" s="17"/>
       <c r="D113" s="17"/>
       <c r="E113" s="17"/>
       <c r="F113" s="17"/>
       <c r="G113" s="17"/>
     </row>
-    <row r="114" spans="3:7" x14ac:dyDescent="0.3">
+    <row r="114" spans="3:7">
       <c r="C114" s="17"/>
       <c r="D114" s="17"/>
       <c r="E114" s="17"/>
@@ -5499,7 +5402,8 @@
       <c r="G114" s="17"/>
     </row>
   </sheetData>
-  <mergeCells count="40">
+  <mergeCells count="41">
+    <mergeCell ref="Q62:Q68"/>
     <mergeCell ref="I62:I78"/>
     <mergeCell ref="A62:A78"/>
     <mergeCell ref="A37:A53"/>
@@ -5550,20 +5454,20 @@
       <controls>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1038" r:id="rId4" name="Scroll Bar 14">
-              <controlPr defaultSize="0" autoPict="0" macro="[0]!ScrollBar14_Change">
-                <anchor moveWithCells="1">
+            <control shapeId="1044" r:id="rId4" name="Spinner 20">
+              <controlPr defaultSize="0" autoPict="0">
+                <anchor moveWithCells="1" sizeWithCells="1">
                   <from>
-                    <xdr:col>23</xdr:col>
-                    <xdr:colOff>83820</xdr:colOff>
-                    <xdr:row>28</xdr:row>
-                    <xdr:rowOff>0</xdr:rowOff>
+                    <xdr:col>25</xdr:col>
+                    <xdr:colOff>47625</xdr:colOff>
+                    <xdr:row>29</xdr:row>
+                    <xdr:rowOff>47625</xdr:rowOff>
                   </from>
                   <to>
-                    <xdr:col>23</xdr:col>
-                    <xdr:colOff>556260</xdr:colOff>
-                    <xdr:row>45</xdr:row>
-                    <xdr:rowOff>106680</xdr:rowOff>
+                    <xdr:col>25</xdr:col>
+                    <xdr:colOff>542925</xdr:colOff>
+                    <xdr:row>36</xdr:row>
+                    <xdr:rowOff>66675</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>
@@ -5572,20 +5476,20 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1039" r:id="rId5" name="Scroll Bar 15">
-              <controlPr defaultSize="0" autoPict="0" macro="[0]!ScrollBar14_Change">
-                <anchor moveWithCells="1">
+            <control shapeId="1046" r:id="rId5" name="Spinner 22">
+              <controlPr defaultSize="0" autoPict="0">
+                <anchor moveWithCells="1" sizeWithCells="1">
                   <from>
-                    <xdr:col>24</xdr:col>
-                    <xdr:colOff>76200</xdr:colOff>
-                    <xdr:row>27</xdr:row>
-                    <xdr:rowOff>190500</xdr:rowOff>
+                    <xdr:col>26</xdr:col>
+                    <xdr:colOff>66675</xdr:colOff>
+                    <xdr:row>29</xdr:row>
+                    <xdr:rowOff>47625</xdr:rowOff>
                   </from>
                   <to>
-                    <xdr:col>24</xdr:col>
-                    <xdr:colOff>525780</xdr:colOff>
-                    <xdr:row>45</xdr:row>
-                    <xdr:rowOff>99060</xdr:rowOff>
+                    <xdr:col>26</xdr:col>
+                    <xdr:colOff>552450</xdr:colOff>
+                    <xdr:row>36</xdr:row>
+                    <xdr:rowOff>76200</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>
@@ -5594,20 +5498,20 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1040" r:id="rId6" name="Scroll Bar 16">
-              <controlPr defaultSize="0" autoPict="0" macro="[0]!ScrollBar14_Change">
-                <anchor moveWithCells="1">
+            <control shapeId="1047" r:id="rId6" name="Spinner 23">
+              <controlPr defaultSize="0" autoPict="0">
+                <anchor moveWithCells="1" sizeWithCells="1">
                   <from>
-                    <xdr:col>25</xdr:col>
-                    <xdr:colOff>83820</xdr:colOff>
-                    <xdr:row>28</xdr:row>
-                    <xdr:rowOff>0</xdr:rowOff>
+                    <xdr:col>27</xdr:col>
+                    <xdr:colOff>57150</xdr:colOff>
+                    <xdr:row>29</xdr:row>
+                    <xdr:rowOff>47625</xdr:rowOff>
                   </from>
                   <to>
-                    <xdr:col>25</xdr:col>
-                    <xdr:colOff>541020</xdr:colOff>
-                    <xdr:row>45</xdr:row>
-                    <xdr:rowOff>99060</xdr:rowOff>
+                    <xdr:col>27</xdr:col>
+                    <xdr:colOff>542925</xdr:colOff>
+                    <xdr:row>36</xdr:row>
+                    <xdr:rowOff>66675</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>
@@ -5616,20 +5520,20 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1041" r:id="rId7" name="Scroll Bar 17">
-              <controlPr defaultSize="0" autoPict="0" macro="[0]!ScrollBar14_Change">
-                <anchor moveWithCells="1">
+            <control shapeId="1048" r:id="rId7" name="Spinner 24">
+              <controlPr defaultSize="0" autoPict="0">
+                <anchor moveWithCells="1" sizeWithCells="1">
                   <from>
-                    <xdr:col>26</xdr:col>
-                    <xdr:colOff>83820</xdr:colOff>
-                    <xdr:row>28</xdr:row>
-                    <xdr:rowOff>0</xdr:rowOff>
+                    <xdr:col>28</xdr:col>
+                    <xdr:colOff>47625</xdr:colOff>
+                    <xdr:row>29</xdr:row>
+                    <xdr:rowOff>47625</xdr:rowOff>
                   </from>
                   <to>
-                    <xdr:col>26</xdr:col>
+                    <xdr:col>28</xdr:col>
                     <xdr:colOff>533400</xdr:colOff>
-                    <xdr:row>45</xdr:row>
-                    <xdr:rowOff>99060</xdr:rowOff>
+                    <xdr:row>36</xdr:row>
+                    <xdr:rowOff>66675</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>
@@ -5638,20 +5542,20 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1042" r:id="rId8" name="Scroll Bar 18">
-              <controlPr defaultSize="0" autoPict="0" macro="[0]!ScrollBar14_Change">
-                <anchor moveWithCells="1">
+            <control shapeId="1049" r:id="rId8" name="Spinner 25">
+              <controlPr defaultSize="0" autoPict="0">
+                <anchor moveWithCells="1" sizeWithCells="1">
                   <from>
-                    <xdr:col>27</xdr:col>
-                    <xdr:colOff>68580</xdr:colOff>
-                    <xdr:row>27</xdr:row>
-                    <xdr:rowOff>190500</xdr:rowOff>
+                    <xdr:col>24</xdr:col>
+                    <xdr:colOff>66675</xdr:colOff>
+                    <xdr:row>29</xdr:row>
+                    <xdr:rowOff>47625</xdr:rowOff>
                   </from>
                   <to>
-                    <xdr:col>27</xdr:col>
-                    <xdr:colOff>525780</xdr:colOff>
-                    <xdr:row>45</xdr:row>
-                    <xdr:rowOff>99060</xdr:rowOff>
+                    <xdr:col>24</xdr:col>
+                    <xdr:colOff>542925</xdr:colOff>
+                    <xdr:row>36</xdr:row>
+                    <xdr:rowOff>66675</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>
@@ -5660,152 +5564,20 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1043" r:id="rId9" name="Scroll Bar 19">
-              <controlPr defaultSize="0" autoPict="0" macro="[0]!ScrollBar14_Change">
-                <anchor moveWithCells="1">
-                  <from>
-                    <xdr:col>28</xdr:col>
-                    <xdr:colOff>60960</xdr:colOff>
-                    <xdr:row>28</xdr:row>
-                    <xdr:rowOff>0</xdr:rowOff>
-                  </from>
-                  <to>
-                    <xdr:col>28</xdr:col>
-                    <xdr:colOff>518160</xdr:colOff>
-                    <xdr:row>45</xdr:row>
-                    <xdr:rowOff>99060</xdr:rowOff>
-                  </to>
-                </anchor>
-              </controlPr>
-            </control>
-          </mc:Choice>
-        </mc:AlternateContent>
-        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-          <mc:Choice Requires="x14">
-            <control shapeId="1044" r:id="rId10" name="Spinner 20">
-              <controlPr defaultSize="0" autoPict="0">
-                <anchor moveWithCells="1" sizeWithCells="1">
-                  <from>
-                    <xdr:col>25</xdr:col>
-                    <xdr:colOff>60960</xdr:colOff>
-                    <xdr:row>49</xdr:row>
-                    <xdr:rowOff>190500</xdr:rowOff>
-                  </from>
-                  <to>
-                    <xdr:col>25</xdr:col>
-                    <xdr:colOff>548640</xdr:colOff>
-                    <xdr:row>57</xdr:row>
-                    <xdr:rowOff>22860</xdr:rowOff>
-                  </to>
-                </anchor>
-              </controlPr>
-            </control>
-          </mc:Choice>
-        </mc:AlternateContent>
-        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-          <mc:Choice Requires="x14">
-            <control shapeId="1046" r:id="rId11" name="Spinner 22">
-              <controlPr defaultSize="0" autoPict="0">
-                <anchor moveWithCells="1" sizeWithCells="1">
-                  <from>
-                    <xdr:col>26</xdr:col>
-                    <xdr:colOff>76200</xdr:colOff>
-                    <xdr:row>50</xdr:row>
-                    <xdr:rowOff>0</xdr:rowOff>
-                  </from>
-                  <to>
-                    <xdr:col>26</xdr:col>
-                    <xdr:colOff>563880</xdr:colOff>
-                    <xdr:row>57</xdr:row>
-                    <xdr:rowOff>30480</xdr:rowOff>
-                  </to>
-                </anchor>
-              </controlPr>
-            </control>
-          </mc:Choice>
-        </mc:AlternateContent>
-        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-          <mc:Choice Requires="x14">
-            <control shapeId="1047" r:id="rId12" name="Spinner 23">
-              <controlPr defaultSize="0" autoPict="0">
-                <anchor moveWithCells="1" sizeWithCells="1">
-                  <from>
-                    <xdr:col>27</xdr:col>
-                    <xdr:colOff>68580</xdr:colOff>
-                    <xdr:row>49</xdr:row>
-                    <xdr:rowOff>190500</xdr:rowOff>
-                  </from>
-                  <to>
-                    <xdr:col>27</xdr:col>
-                    <xdr:colOff>548640</xdr:colOff>
-                    <xdr:row>57</xdr:row>
-                    <xdr:rowOff>22860</xdr:rowOff>
-                  </to>
-                </anchor>
-              </controlPr>
-            </control>
-          </mc:Choice>
-        </mc:AlternateContent>
-        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-          <mc:Choice Requires="x14">
-            <control shapeId="1048" r:id="rId13" name="Spinner 24">
-              <controlPr defaultSize="0" autoPict="0">
-                <anchor moveWithCells="1" sizeWithCells="1">
-                  <from>
-                    <xdr:col>28</xdr:col>
-                    <xdr:colOff>60960</xdr:colOff>
-                    <xdr:row>50</xdr:row>
-                    <xdr:rowOff>0</xdr:rowOff>
-                  </from>
-                  <to>
-                    <xdr:col>28</xdr:col>
-                    <xdr:colOff>541020</xdr:colOff>
-                    <xdr:row>57</xdr:row>
-                    <xdr:rowOff>22860</xdr:rowOff>
-                  </to>
-                </anchor>
-              </controlPr>
-            </control>
-          </mc:Choice>
-        </mc:AlternateContent>
-        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-          <mc:Choice Requires="x14">
-            <control shapeId="1049" r:id="rId14" name="Spinner 25">
-              <controlPr defaultSize="0" autoPict="0">
-                <anchor moveWithCells="1" sizeWithCells="1">
-                  <from>
-                    <xdr:col>24</xdr:col>
-                    <xdr:colOff>76200</xdr:colOff>
-                    <xdr:row>49</xdr:row>
-                    <xdr:rowOff>190500</xdr:rowOff>
-                  </from>
-                  <to>
-                    <xdr:col>24</xdr:col>
-                    <xdr:colOff>556260</xdr:colOff>
-                    <xdr:row>57</xdr:row>
-                    <xdr:rowOff>22860</xdr:rowOff>
-                  </to>
-                </anchor>
-              </controlPr>
-            </control>
-          </mc:Choice>
-        </mc:AlternateContent>
-        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-          <mc:Choice Requires="x14">
-            <control shapeId="1050" r:id="rId15" name="Spinner 26">
+            <control shapeId="1050" r:id="rId9" name="Spinner 26">
               <controlPr defaultSize="0" autoPict="0">
                 <anchor moveWithCells="1" sizeWithCells="1">
                   <from>
                     <xdr:col>23</xdr:col>
-                    <xdr:colOff>91440</xdr:colOff>
-                    <xdr:row>50</xdr:row>
-                    <xdr:rowOff>0</xdr:rowOff>
+                    <xdr:colOff>85725</xdr:colOff>
+                    <xdr:row>29</xdr:row>
+                    <xdr:rowOff>47625</xdr:rowOff>
                   </from>
                   <to>
                     <xdr:col>23</xdr:col>
-                    <xdr:colOff>571500</xdr:colOff>
-                    <xdr:row>57</xdr:row>
-                    <xdr:rowOff>22860</xdr:rowOff>
+                    <xdr:colOff>561975</xdr:colOff>
+                    <xdr:row>36</xdr:row>
+                    <xdr:rowOff>66675</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>

</xml_diff>